<commit_message>
I noticed that some pH values didn't average all three replicates in the mean. I updated them.
</commit_message>
<xml_diff>
--- a/check sample work/pH QAQC/20210326 pH check sample results summary.xlsx
+++ b/check sample work/pH QAQC/20210326 pH check sample results summary.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\915712257\Documents\R\rye-tech-sfsu\2021-season-summary\check sample work\pH QAQC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rye-Tech\Documents\R\rye-tech-home\2021-season-summary\check sample work\pH QAQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A54FF7-D474-46A3-85FE-6DC4DD0F7A8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20736" windowHeight="11160" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="example to follow" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'pH samples jul 2018 nov 2020'!$A$1:$O$191</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -977,7 +978,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -1643,27 +1644,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
-    <col min="13" max="13" width="51.109375" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="13" max="13" width="51.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1701,7 +1702,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1715,7 +1716,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1726,7 +1727,7 @@
         <v>2247.5363699999998</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1770,7 +1771,7 @@
       </c>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1781,7 +1782,7 @@
         <v>2114.1481899999999</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1792,7 +1793,7 @@
         <v>2138.9193500000001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1836,7 +1837,7 @@
       </c>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1847,7 +1848,7 @@
         <v>2135.2389699999999</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1858,7 +1859,7 @@
         <v>2133.48756</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1902,7 +1903,7 @@
       </c>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1913,7 +1914,7 @@
         <v>2124.9360900000001</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1924,7 +1925,7 @@
         <v>2132.3921700000001</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1968,7 +1969,7 @@
       </c>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1979,7 +1980,7 @@
         <v>2249.3508299999999</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1990,7 +1991,7 @@
         <v>2250.2915600000001</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2037,10 +2038,10 @@
       </c>
       <c r="M16" s="3"/>
     </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
       <c r="N20" s="4"/>
     </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>34</v>
       </c>
@@ -2051,7 +2052,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E22">
         <f>2238.04</f>
         <v>2238.04</v>
@@ -2065,7 +2066,7 @@
         <v>21.704231088401922</v>
       </c>
     </row>
-    <row r="23" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E23">
         <f t="shared" ref="E23:E26" si="0">2238.04</f>
         <v>2238.04</v>
@@ -2079,7 +2080,7 @@
         <v>90.181043176897006</v>
       </c>
     </row>
-    <row r="24" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E24">
         <f t="shared" si="0"/>
         <v>2238.04</v>
@@ -2093,7 +2094,7 @@
         <v>62.986127504401573</v>
       </c>
     </row>
-    <row r="25" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E25">
         <f>2238.04</f>
         <v>2238.04</v>
@@ -2107,7 +2108,7 @@
         <v>127.93487528889766</v>
       </c>
     </row>
-    <row r="26" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E26">
         <f t="shared" si="0"/>
         <v>2238.04</v>
@@ -2121,7 +2122,7 @@
         <v>150.10072243360378</v>
       </c>
     </row>
-    <row r="29" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:14" x14ac:dyDescent="0.25">
       <c r="G29">
         <f>SQRT(SUM(G22:G26)/5)</f>
         <v>9.5174261173092578</v>
@@ -2130,7 +2131,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F30" s="3"/>
       <c r="G30">
         <v>0.53</v>
@@ -2139,7 +2140,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:14" x14ac:dyDescent="0.25">
       <c r="G31">
         <f>SQRT(G29^2+G30^2)</f>
         <v>9.5321718353395397</v>
@@ -2151,7 +2152,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:14" x14ac:dyDescent="0.25">
       <c r="G32">
         <f>G31/E26</f>
         <v>4.2591606206053246E-3</v>
@@ -2163,12 +2164,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:13" x14ac:dyDescent="0.25">
       <c r="M36" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="4:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:13" ht="45" x14ac:dyDescent="0.25">
       <c r="D37" s="1" t="s">
         <v>38</v>
       </c>
@@ -2180,30 +2181,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K242" sqref="K242"/>
+      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G255" activeCellId="2" sqref="G249 G252 G255"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.88671875" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.88671875" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="13" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="14" customWidth="1"/>
     <col min="11" max="14" width="13" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="51.109375" style="17" customWidth="1"/>
-    <col min="16" max="16384" width="9.109375" style="17"/>
+    <col min="15" max="15" width="51.140625" style="17" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2247,7 +2248,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>50</v>
       </c>
@@ -2262,7 +2263,7 @@
         <v>7.74153486291614</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>51</v>
       </c>
@@ -2309,7 +2310,7 @@
         <v>9.4507647610004852E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>52</v>
       </c>
@@ -2330,7 +2331,7 @@
       <c r="K4" s="19"/>
       <c r="O4" s="20"/>
     </row>
-    <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>53</v>
       </c>
@@ -2344,7 +2345,7 @@
         <v>8.0789632362488106</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>55</v>
       </c>
@@ -2390,7 +2391,7 @@
         <v>9.9640870000001769E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>56</v>
       </c>
@@ -2404,7 +2405,7 @@
         <v>7.8272875099999997</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>57</v>
       </c>
@@ -2424,7 +2425,7 @@
       <c r="K8" s="19"/>
       <c r="O8" s="20"/>
     </row>
-    <row r="9" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>58</v>
       </c>
@@ -2444,7 +2445,7 @@
       <c r="K9" s="19"/>
       <c r="O9" s="20"/>
     </row>
-    <row r="10" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>59</v>
       </c>
@@ -2464,7 +2465,7 @@
       <c r="K10" s="19"/>
       <c r="O10" s="20"/>
     </row>
-    <row r="11" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>60</v>
       </c>
@@ -2484,7 +2485,7 @@
       <c r="K11" s="19"/>
       <c r="O11" s="20"/>
     </row>
-    <row r="12" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>61</v>
       </c>
@@ -2504,7 +2505,7 @@
       <c r="K12" s="19"/>
       <c r="O12" s="20"/>
     </row>
-    <row r="13" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>62</v>
       </c>
@@ -2551,7 +2552,7 @@
       </c>
       <c r="O13" s="20"/>
     </row>
-    <row r="14" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>63</v>
       </c>
@@ -2571,7 +2572,7 @@
       <c r="K14" s="19"/>
       <c r="O14" s="20"/>
     </row>
-    <row r="15" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>64</v>
       </c>
@@ -2591,7 +2592,7 @@
       <c r="K15" s="19"/>
       <c r="O15" s="20"/>
     </row>
-    <row r="16" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>65</v>
       </c>
@@ -2611,7 +2612,7 @@
       <c r="K16" s="19"/>
       <c r="O16" s="20"/>
     </row>
-    <row r="17" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>66</v>
       </c>
@@ -2625,7 +2626,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>67</v>
       </c>
@@ -2639,7 +2640,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>68</v>
       </c>
@@ -2653,7 +2654,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>69</v>
       </c>
@@ -2667,7 +2668,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>70</v>
       </c>
@@ -2681,7 +2682,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>71</v>
       </c>
@@ -2727,7 +2728,7 @@
         <v>5.4133608872302119E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>72</v>
       </c>
@@ -2741,7 +2742,7 @@
         <v>7.7988739523662698</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>73</v>
       </c>
@@ -2755,7 +2756,7 @@
         <v>7.79305526944073</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>74</v>
       </c>
@@ -2801,7 +2802,7 @@
         <v>3.1232441419497547E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>75</v>
       </c>
@@ -2815,7 +2816,7 @@
         <v>7.9540741754416899</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>76</v>
       </c>
@@ -2829,7 +2830,7 @@
         <v>7.9594204270895696</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>77</v>
       </c>
@@ -2843,7 +2844,7 @@
         <v>8.0873331962983404</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>78</v>
       </c>
@@ -2889,7 +2890,7 @@
         <v>1.0720631408151604E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>79</v>
       </c>
@@ -2903,7 +2904,7 @@
         <v>7.9935739879872703</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>80</v>
       </c>
@@ -2917,7 +2918,7 @@
         <v>7.9966718658117797</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>81</v>
       </c>
@@ -2963,7 +2964,7 @@
         <v>2.2264576316979756E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>82</v>
       </c>
@@ -2977,7 +2978,7 @@
         <v>7.8397113904705504</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>83</v>
       </c>
@@ -2991,7 +2992,7 @@
         <v>7.8274796640885898</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>44</v>
       </c>
@@ -3038,7 +3039,7 @@
         <v>2.2439329999999202E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>45</v>
       </c>
@@ -3053,7 +3054,7 @@
         <v>7.6206292969999998</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>46</v>
       </c>
@@ -3074,7 +3075,7 @@
       <c r="K37" s="19"/>
       <c r="O37" s="20"/>
     </row>
-    <row r="38" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>84</v>
       </c>
@@ -3120,7 +3121,7 @@
         <v>1.0153592664430278E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>85</v>
       </c>
@@ -3134,7 +3135,7 @@
         <v>7.6916903045289899</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>86</v>
       </c>
@@ -3148,7 +3149,7 @@
         <v>7.69283522006263</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>44</v>
       </c>
@@ -3194,7 +3195,7 @@
         <v>2.2340176990400806E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>45</v>
       </c>
@@ -3208,7 +3209,7 @@
         <v>7.6206853918415103</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>46</v>
       </c>
@@ -3222,7 +3223,7 @@
         <v>7.5723148968455796</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>87</v>
       </c>
@@ -3268,7 +3269,7 @@
         <v>5.4535375515403217E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>88</v>
       </c>
@@ -3282,7 +3283,7 @@
         <v>7.7435457498339</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>89</v>
       </c>
@@ -3296,7 +3297,7 @@
         <v>7.7425531075232099</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>90</v>
       </c>
@@ -3342,7 +3343,7 @@
         <v>1.9462257076501288E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>91</v>
       </c>
@@ -3356,7 +3357,7 @@
         <v>7.85309992140568</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>92</v>
       </c>
@@ -3370,7 +3371,7 @@
         <v>7.8511140300557098</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>93</v>
       </c>
@@ -3384,7 +3385,7 @@
         <v>7.6858002409995496</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>94</v>
       </c>
@@ -3398,7 +3399,7 @@
         <v>7.6604061490644897</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>95</v>
       </c>
@@ -3412,7 +3413,7 @@
         <v>8.0900620266582006</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>96</v>
       </c>
@@ -3426,7 +3427,7 @@
         <v>7.6378195889536498</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>97</v>
       </c>
@@ -3440,7 +3441,7 @@
         <v>7.6496254781234603</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>98</v>
       </c>
@@ -3454,7 +3455,7 @@
         <v>8.0839369011466005</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>99</v>
       </c>
@@ -3500,7 +3501,7 @@
         <v>1.6633850593983368E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>100</v>
       </c>
@@ -3514,7 +3515,7 @@
         <v>7.8860289201581297</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>101</v>
       </c>
@@ -3528,7 +3529,7 @@
         <v>7.8842376073644704</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
         <v>102</v>
       </c>
@@ -3542,7 +3543,7 @@
         <v>8.0814347249955993</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
         <v>144</v>
       </c>
@@ -3560,7 +3561,7 @@
       <c r="L60" s="15"/>
       <c r="M60" s="15"/>
     </row>
-    <row r="61" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
         <v>145</v>
       </c>
@@ -3574,7 +3575,7 @@
         <v>7.1826006600000003</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
         <v>146</v>
       </c>
@@ -3588,7 +3589,7 @@
         <v>7.2032755269999997</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
         <v>131</v>
       </c>
@@ -3602,7 +3603,7 @@
         <v>7.7168752789999999</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
         <v>132</v>
       </c>
@@ -3616,7 +3617,7 @@
         <v>6.0824875330000001</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
         <v>133</v>
       </c>
@@ -3630,7 +3631,7 @@
         <v>7.7928240129999997</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
         <v>134</v>
       </c>
@@ -3644,7 +3645,7 @@
         <v>7.1200401400000004</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
         <v>135</v>
       </c>
@@ -3658,7 +3659,7 @@
         <v>7.6971565870000003</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
         <v>136</v>
       </c>
@@ -3672,7 +3673,7 @@
         <v>7.1042788000000003</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
         <v>123</v>
       </c>
@@ -3718,7 +3719,7 @@
         <v>3.8996199999985492E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
         <v>124</v>
       </c>
@@ -3732,7 +3733,7 @@
         <v>7.7374005620000004</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
         <v>125</v>
       </c>
@@ -3746,7 +3747,7 @@
         <v>7.7393420920000002</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
         <v>126</v>
       </c>
@@ -3760,7 +3761,7 @@
         <v>7.7354182920000003</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
         <v>127</v>
       </c>
@@ -3806,7 +3807,7 @@
         <v>0.14325217900000009</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
         <v>128</v>
       </c>
@@ -3820,7 +3821,7 @@
         <v>7.0702561770000001</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
         <v>129</v>
       </c>
@@ -3834,7 +3835,7 @@
         <v>7.0495923649999996</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
         <v>130</v>
       </c>
@@ -3848,7 +3849,7 @@
         <v>8.0626476389999997</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
         <v>117</v>
       </c>
@@ -3894,7 +3895,7 @@
         <v>6.9391389999999831E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
         <v>118</v>
       </c>
@@ -3908,7 +3909,7 @@
         <v>7.2533112170000003</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
         <v>119</v>
       </c>
@@ -3922,7 +3923,7 @@
         <v>7.2335023679999999</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
         <v>120</v>
       </c>
@@ -3968,7 +3969,7 @@
         <v>3.0759240000000077E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
         <v>121</v>
       </c>
@@ -3982,7 +3983,7 @@
         <v>7.774027029</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
         <v>122</v>
       </c>
@@ -3996,7 +3997,7 @@
         <v>7.7718314790000003</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
         <v>113</v>
       </c>
@@ -4042,7 +4043,7 @@
         <v>5.5175080000005039E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
         <v>114</v>
       </c>
@@ -4056,7 +4057,7 @@
         <v>7.7390057639999998</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
         <v>115</v>
       </c>
@@ -4102,7 +4103,7 @@
         <v>0.39663596199999951</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
         <v>116</v>
       </c>
@@ -4116,7 +4117,7 @@
         <v>6.3836745009999998</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
         <v>137</v>
       </c>
@@ -4162,7 +4163,7 @@
         <v>3.3557309999991958E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
         <v>138</v>
       </c>
@@ -4176,7 +4177,7 @@
         <v>7.8138157469999996</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
         <v>139</v>
       </c>
@@ -4222,7 +4223,7 @@
         <v>3.984354099999976E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
         <v>140</v>
       </c>
@@ -4236,7 +4237,7 @@
         <v>7.1890400999999997</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
         <v>141</v>
       </c>
@@ -4282,7 +4283,7 @@
         <v>1.4239060000003079E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
         <v>142</v>
       </c>
@@ -4296,7 +4297,7 @@
         <v>7.8047359729999997</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
         <v>143</v>
       </c>
@@ -4310,7 +4311,7 @@
         <v>7.7955808449999999</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
         <v>103</v>
       </c>
@@ -4356,7 +4357,7 @@
         <v>2.1472610000001779E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
         <v>104</v>
       </c>
@@ -4370,7 +4371,7 @@
         <v>7.8017914089999998</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
         <v>105</v>
       </c>
@@ -4384,7 +4385,7 @@
         <v>7.8118574880000002</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
         <v>106</v>
       </c>
@@ -4430,7 +4431,7 @@
         <v>2.5400840000004976E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
         <v>107</v>
       </c>
@@ -4444,7 +4445,7 @@
         <v>7.7766032569999997</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
         <v>108</v>
       </c>
@@ -4458,7 +4459,7 @@
         <v>7.78986102</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
         <v>109</v>
       </c>
@@ -4504,7 +4505,7 @@
         <v>4.7052929999997772E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
         <v>110</v>
       </c>
@@ -4518,7 +4519,7 @@
         <v>7.7917906620000004</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
         <v>111</v>
       </c>
@@ -4532,7 +4533,7 @@
         <v>7.7886460780000002</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
         <v>112</v>
       </c>
@@ -4550,7 +4551,7 @@
       <c r="L103" s="15"/>
       <c r="M103" s="15"/>
     </row>
-    <row r="104" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
         <v>147</v>
       </c>
@@ -4596,7 +4597,7 @@
         <v>8.5959990000006314E-3</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
         <v>148</v>
       </c>
@@ -4610,7 +4611,7 @@
         <v>7.6605760270000003</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
         <v>149</v>
       </c>
@@ -4624,7 +4625,7 @@
         <v>7.6567980359999996</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
         <v>150</v>
       </c>
@@ -4670,7 +4671,7 @@
         <v>6.9301700000057309E-4</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
         <v>151</v>
       </c>
@@ -4684,7 +4685,7 @@
         <v>7.6343832159999998</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
         <v>152</v>
       </c>
@@ -4698,7 +4699,7 @@
         <v>7.6326811010000002</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
         <v>153</v>
       </c>
@@ -4712,7 +4713,7 @@
         <v>7.6821010679999997</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
         <v>154</v>
       </c>
@@ -4758,7 +4759,7 @@
         <v>5.6953400000026022E-4</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
         <v>155</v>
       </c>
@@ -4772,7 +4773,7 @@
         <v>7.1364007689999998</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
         <v>156</v>
       </c>
@@ -4786,7 +4787,7 @@
         <v>7.1419704160000004</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
         <v>157</v>
       </c>
@@ -4832,7 +4833,7 @@
         <v>3.9157139999996815E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
         <v>158</v>
       </c>
@@ -4846,7 +4847,7 @@
         <v>7.468608819</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
         <v>159</v>
       </c>
@@ -4860,7 +4861,7 @@
         <v>7.4689537149999996</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
         <v>160</v>
       </c>
@@ -4874,7 +4875,7 @@
         <v>7.6803900140000003</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
         <v>161</v>
       </c>
@@ -4920,7 +4921,7 @@
         <v>4.6619300000028119E-4</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
         <v>162</v>
       </c>
@@ -4934,7 +4935,7 @@
         <v>7.667210173</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
         <v>163</v>
       </c>
@@ -4948,7 +4949,7 @@
         <v>7.6669448720000002</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="14" t="s">
         <v>164</v>
       </c>
@@ -4994,7 +4995,7 @@
         <v>3.2636009999995608E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
         <v>165</v>
       </c>
@@ -5008,7 +5009,7 @@
         <v>7.6536444919999997</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="14" t="s">
         <v>166</v>
       </c>
@@ -5022,7 +5023,7 @@
         <v>7.653440131</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
         <v>167</v>
       </c>
@@ -5068,7 +5069,7 @@
         <v>9.8320349999996282E-3</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
         <v>168</v>
       </c>
@@ -5082,7 +5083,7 @@
         <v>6.3709340689999996</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="14" t="s">
         <v>169</v>
       </c>
@@ -5096,7 +5097,7 @@
         <v>6.3726452409999998</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="21" t="s">
         <v>170</v>
       </c>
@@ -5111,7 +5112,7 @@
         <v>6.9959126630000004</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="14" t="s">
         <v>171</v>
       </c>
@@ -5125,7 +5126,7 @@
         <v>7.6741815879999997</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="14" t="s">
         <v>172</v>
       </c>
@@ -5171,7 +5172,7 @@
         <v>1.7411190000000687E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="14" t="s">
         <v>173</v>
       </c>
@@ -5185,7 +5186,7 @@
         <v>7.6514540369999997</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="14" t="s">
         <v>174</v>
       </c>
@@ -5199,7 +5200,7 @@
         <v>7.6515557080000001</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="14" t="s">
         <v>175</v>
       </c>
@@ -5213,7 +5214,7 @@
         <v>7.316864421</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="14" t="s">
         <v>176</v>
       </c>
@@ -5227,7 +5228,7 @@
         <v>7.9479927589999999</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="14" t="s">
         <v>177</v>
       </c>
@@ -5241,7 +5242,7 @@
         <v>7.6949174229999997</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="14" t="s">
         <v>178</v>
       </c>
@@ -5287,7 +5288,7 @@
         <v>1.1478880999999497E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="14" t="s">
         <v>179</v>
       </c>
@@ -5301,7 +5302,7 @@
         <v>7.6843401650000001</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="14" t="s">
         <v>180</v>
       </c>
@@ -5315,7 +5316,7 @@
         <v>7.6786753970000001</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
         <v>181</v>
       </c>
@@ -5361,7 +5362,7 @@
         <v>4.9260399999999649E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="14" t="s">
         <v>182</v>
       </c>
@@ -5375,7 +5376,7 @@
         <v>7.6961760779999997</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
         <v>183</v>
       </c>
@@ -5389,7 +5390,7 @@
         <v>7.6928150100000003</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
         <v>184</v>
       </c>
@@ -5435,7 +5436,7 @@
         <v>2.6524429999996713E-3</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
         <v>185</v>
       </c>
@@ -5449,7 +5450,7 @@
         <v>7.6982832630000004</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="14" t="s">
         <v>186</v>
       </c>
@@ -5463,7 +5464,7 @@
         <v>7.7082846360000001</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="14" t="s">
         <v>187</v>
       </c>
@@ -5477,7 +5478,7 @@
         <v>7.7066703499999996</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="14" t="s">
         <v>188</v>
       </c>
@@ -5526,7 +5527,7 @@
         <v>7.3740243496089874E-4</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="14" t="s">
         <v>189</v>
       </c>
@@ -5543,7 +5544,7 @@
         <v>7.9539157263998002</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="14" t="s">
         <v>190</v>
       </c>
@@ -5560,7 +5561,7 @@
         <v>7.9573810731919297</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="14" t="s">
         <v>191</v>
       </c>
@@ -5609,7 +5610,7 @@
         <v>5.9682269996397252E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="14" t="s">
         <v>192</v>
       </c>
@@ -5626,7 +5627,7 @@
         <v>8.0261779270012301</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="14" t="s">
         <v>193</v>
       </c>
@@ -5643,7 +5644,7 @@
         <v>8.0209223405981191</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="14" t="s">
         <v>194</v>
       </c>
@@ -5692,7 +5693,7 @@
         <v>9.7571513074896643E-3</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="14" t="s">
         <v>195</v>
       </c>
@@ -5709,7 +5710,7 @@
         <v>8.0421553587913301</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="14" t="s">
         <v>196</v>
       </c>
@@ -5726,7 +5727,7 @@
         <v>8.0358138115455393</v>
       </c>
     </row>
-    <row r="154" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="14" t="s">
         <v>239</v>
       </c>
@@ -5743,7 +5744,7 @@
         <v>7.67031134315069</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="14" t="s">
         <v>197</v>
       </c>
@@ -5760,7 +5761,7 @@
         <v>8.0745769128785891</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="14" t="s">
         <v>198</v>
       </c>
@@ -5809,7 +5810,7 @@
         <v>2.0513919882203524E-3</v>
       </c>
     </row>
-    <row r="157" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="14" t="s">
         <v>199</v>
       </c>
@@ -5826,7 +5827,7 @@
         <v>7.6355414113303102</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="14" t="s">
         <v>200</v>
       </c>
@@ -5843,7 +5844,7 @@
         <v>7.6379501987185598</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="14" t="s">
         <v>240</v>
       </c>
@@ -5860,7 +5861,7 @@
         <v>7.6830802104558602</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="14" t="s">
         <v>201</v>
       </c>
@@ -5909,7 +5910,7 @@
         <v>2.399748012149594E-3</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="14" t="s">
         <v>202</v>
       </c>
@@ -5926,7 +5927,7 @@
         <v>7.6469616334670096</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="14" t="s">
         <v>203</v>
       </c>
@@ -5943,7 +5944,7 @@
         <v>7.6495853108169101</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="14" t="s">
         <v>204</v>
       </c>
@@ -5963,7 +5964,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="14" t="s">
         <v>205</v>
       </c>
@@ -5983,7 +5984,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="14" t="s">
         <v>208</v>
       </c>
@@ -6029,7 +6030,7 @@
         <v>3.8811856922595922E-3</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="14" t="s">
         <v>209</v>
       </c>
@@ -6043,7 +6044,7 @@
         <v>7.8158333436642904</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="14" t="s">
         <v>210</v>
       </c>
@@ -6089,7 +6090,7 @@
         <v>6.0021903599061233E-4</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="14" t="s">
         <v>211</v>
       </c>
@@ -6103,7 +6104,7 @@
         <v>7.8559850453043403</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="14" t="s">
         <v>212</v>
       </c>
@@ -6149,7 +6150,7 @@
         <v>6.8963092720952801E-4</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="14" t="s">
         <v>213</v>
       </c>
@@ -6163,7 +6164,7 @@
         <v>7.8611367023104597</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="14" t="s">
         <v>214</v>
       </c>
@@ -6209,7 +6210,7 @@
         <v>2.3053612821302139E-3</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="14" t="s">
         <v>215</v>
       </c>
@@ -6223,7 +6224,7 @@
         <v>7.8656749752011397</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="14" t="s">
         <v>225</v>
       </c>
@@ -6241,7 +6242,7 @@
       <c r="L173" s="15"/>
       <c r="M173" s="15"/>
     </row>
-    <row r="174" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="14" t="s">
         <v>216</v>
       </c>
@@ -6287,7 +6288,7 @@
         <v>1.6735989730900513E-3</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="14" t="s">
         <v>217</v>
       </c>
@@ -6301,7 +6302,7 @@
         <v>7.8658232744760301</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="14" t="s">
         <v>218</v>
       </c>
@@ -6347,7 +6348,7 @@
         <v>1.5296409123903842E-3</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="14" t="s">
         <v>219</v>
       </c>
@@ -6361,7 +6362,7 @@
         <v>7.7910625496787098</v>
       </c>
     </row>
-    <row r="178" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="14" t="s">
         <v>220</v>
       </c>
@@ -6407,7 +6408,7 @@
         <v>6.2976206001152946E-6</v>
       </c>
     </row>
-    <row r="179" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="14" t="s">
         <v>221</v>
       </c>
@@ -6421,7 +6422,7 @@
         <v>7.77674822365426</v>
       </c>
     </row>
-    <row r="180" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="14" t="s">
         <v>222</v>
       </c>
@@ -6470,7 +6471,7 @@
         <v>5.3144091276100092E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="14" t="s">
         <v>223</v>
       </c>
@@ -6487,7 +6488,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="182" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="14" t="s">
         <v>226</v>
       </c>
@@ -6504,7 +6505,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="183" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="14" t="s">
         <v>224</v>
       </c>
@@ -6518,7 +6519,7 @@
         <v>7.86089245271185</v>
       </c>
     </row>
-    <row r="184" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="14" t="s">
         <v>226</v>
       </c>
@@ -6536,7 +6537,7 @@
       <c r="L184" s="15"/>
       <c r="M184" s="15"/>
     </row>
-    <row r="185" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="14" t="s">
         <v>227</v>
       </c>
@@ -6582,7 +6583,7 @@
         <v>1.7011204008694492E-3</v>
       </c>
     </row>
-    <row r="186" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="14" t="s">
         <v>228</v>
       </c>
@@ -6596,7 +6597,7 @@
         <v>7.8202712500762397</v>
       </c>
     </row>
-    <row r="187" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="14" t="s">
         <v>229</v>
       </c>
@@ -6642,7 +6643,7 @@
         <v>2.9082277420729774E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="14" t="s">
         <v>230</v>
       </c>
@@ -6656,7 +6657,7 @@
         <v>7.87404002677488</v>
       </c>
     </row>
-    <row r="189" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="14" t="s">
         <v>231</v>
       </c>
@@ -6702,7 +6703,7 @@
         <v>2.6729756152799489E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="14" t="s">
         <v>232</v>
       </c>
@@ -6716,7 +6717,7 @@
         <v>7.8471181750488697</v>
       </c>
     </row>
-    <row r="191" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="14" t="s">
         <v>233</v>
       </c>
@@ -6762,7 +6763,7 @@
         <v>5.3888669986097426E-3</v>
       </c>
     </row>
-    <row r="192" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="14" t="s">
         <v>234</v>
       </c>
@@ -6776,7 +6777,7 @@
         <v>7.7813583054262701</v>
       </c>
     </row>
-    <row r="193" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="14" t="s">
         <v>248</v>
       </c>
@@ -6822,7 +6823,7 @@
         <v>2.8102638491498411E-3</v>
       </c>
     </row>
-    <row r="194" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="14" t="s">
         <v>249</v>
       </c>
@@ -6836,7 +6837,7 @@
         <v>7.7568912448131098</v>
       </c>
     </row>
-    <row r="195" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="14" t="s">
         <v>250</v>
       </c>
@@ -6882,7 +6883,7 @@
         <v>1.9084552613604089E-3</v>
       </c>
     </row>
-    <row r="196" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="14" t="s">
         <v>251</v>
       </c>
@@ -6896,7 +6897,7 @@
         <v>7.8733900677320703</v>
       </c>
     </row>
-    <row r="197" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="14" t="s">
         <v>252</v>
       </c>
@@ -6942,7 +6943,7 @@
         <v>2.0846582444002948E-3</v>
       </c>
     </row>
-    <row r="198" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="14" t="s">
         <v>253</v>
       </c>
@@ -6956,7 +6957,7 @@
         <v>7.7263978191714298</v>
       </c>
     </row>
-    <row r="199" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="14" t="s">
         <v>254</v>
       </c>
@@ -7002,7 +7003,7 @@
         <v>3.3138559194894057E-3</v>
       </c>
     </row>
-    <row r="200" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="14" t="s">
         <v>255</v>
       </c>
@@ -7016,7 +7017,7 @@
         <v>7.7624872040259403</v>
       </c>
     </row>
-    <row r="201" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="14" t="s">
         <v>265</v>
       </c>
@@ -7030,7 +7031,7 @@
         <v>7.7065716469648402</v>
       </c>
     </row>
-    <row r="202" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="14" t="s">
         <v>256</v>
       </c>
@@ -7076,7 +7077,7 @@
         <v>2.4641745023901152E-3</v>
       </c>
     </row>
-    <row r="203" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="14" t="s">
         <v>257</v>
       </c>
@@ -7090,7 +7091,7 @@
         <v>7.7295066813725404</v>
       </c>
     </row>
-    <row r="204" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="14" t="s">
         <v>258</v>
       </c>
@@ -7136,7 +7137,7 @@
         <v>1.8364403182902223E-3</v>
       </c>
     </row>
-    <row r="205" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="14" t="s">
         <v>259</v>
       </c>
@@ -7150,7 +7151,7 @@
         <v>7.7135628084406003</v>
       </c>
     </row>
-    <row r="206" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="14" t="s">
         <v>260</v>
       </c>
@@ -7196,7 +7197,7 @@
         <v>7.1404976746798354E-3</v>
       </c>
     </row>
-    <row r="207" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="14" t="s">
         <v>261</v>
       </c>
@@ -7210,7 +7211,7 @@
         <v>7.78548679949935</v>
       </c>
     </row>
-    <row r="208" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="14" t="s">
         <v>262</v>
       </c>
@@ -7256,7 +7257,7 @@
         <v>1.5627490742886607E-3</v>
       </c>
     </row>
-    <row r="209" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="14" t="s">
         <v>263</v>
       </c>
@@ -7270,7 +7271,7 @@
         <v>7.9116433615381201</v>
       </c>
     </row>
-    <row r="210" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="14" t="s">
         <v>264</v>
       </c>
@@ -7284,7 +7285,7 @@
         <v>7.7210421811258003</v>
       </c>
     </row>
-    <row r="211" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A211" s="14" t="s">
         <v>266</v>
       </c>
@@ -7333,7 +7334,7 @@
         <v>0.1854344769760301</v>
       </c>
     </row>
-    <row r="212" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="14" t="s">
         <v>267</v>
       </c>
@@ -7350,7 +7351,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="213" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="14" t="s">
         <v>268</v>
       </c>
@@ -7399,7 +7400,7 @@
         <v>0.19568697425110049</v>
       </c>
     </row>
-    <row r="214" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="14" t="s">
         <v>269</v>
       </c>
@@ -7416,7 +7417,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="215" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A215" s="14" t="s">
         <v>270</v>
       </c>
@@ -7465,7 +7466,7 @@
         <v>3.6690036611499721E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A216" s="14" t="s">
         <v>271</v>
       </c>
@@ -7482,7 +7483,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="217" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="14" t="s">
         <v>272</v>
       </c>
@@ -7531,7 +7532,7 @@
         <v>2.9172948538660037E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" s="14" t="s">
         <v>273</v>
       </c>
@@ -7548,7 +7549,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="219" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" s="14" t="s">
         <v>274</v>
       </c>
@@ -7565,7 +7566,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="220" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A220" s="14" t="s">
         <v>276</v>
       </c>
@@ -7614,7 +7615,7 @@
         <v>7.1857585881370589E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="14" t="s">
         <v>277</v>
       </c>
@@ -7631,7 +7632,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="222" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A222" s="14" t="s">
         <v>278</v>
       </c>
@@ -7680,7 +7681,7 @@
         <v>5.7847597330809464E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A223" s="14" t="s">
         <v>279</v>
       </c>
@@ -7697,7 +7698,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="224" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A224" s="14" t="s">
         <v>280</v>
       </c>
@@ -7746,7 +7747,7 @@
         <v>0.2161789027148604</v>
       </c>
     </row>
-    <row r="225" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A225" s="14" t="s">
         <v>281</v>
       </c>
@@ -7763,7 +7764,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="226" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A226" s="14" t="s">
         <v>282</v>
       </c>
@@ -7812,7 +7813,7 @@
         <v>3.847784957223066E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="14" t="s">
         <v>283</v>
       </c>
@@ -7829,7 +7830,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="228" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" s="14" t="s">
         <v>284</v>
       </c>
@@ -7846,7 +7847,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="229" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="14" t="s">
         <v>285</v>
       </c>
@@ -7892,7 +7893,7 @@
         <v>9.2158552030479512E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="14" t="s">
         <v>286</v>
       </c>
@@ -7906,7 +7907,7 @@
         <v>7.6791676929657999</v>
       </c>
     </row>
-    <row r="231" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="14" t="s">
         <v>287</v>
       </c>
@@ -7952,7 +7953,7 @@
         <v>1.6493493007419424E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="14" t="s">
         <v>288</v>
       </c>
@@ -7966,7 +7967,7 @@
         <v>7.6709188894545699</v>
       </c>
     </row>
-    <row r="233" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="14" t="s">
         <v>289</v>
       </c>
@@ -8012,7 +8013,7 @@
         <v>2.514442181299259E-3</v>
       </c>
     </row>
-    <row r="234" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="14" t="s">
         <v>290</v>
       </c>
@@ -8026,7 +8027,7 @@
         <v>7.8598848256278</v>
       </c>
     </row>
-    <row r="235" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="14" t="s">
         <v>291</v>
       </c>
@@ -8072,7 +8073,7 @@
         <v>2.7849821903496164E-3</v>
       </c>
     </row>
-    <row r="236" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="14" t="s">
         <v>292</v>
       </c>
@@ -8086,7 +8087,7 @@
         <v>7.8379624344456804</v>
       </c>
     </row>
-    <row r="237" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="14" t="s">
         <v>293</v>
       </c>
@@ -8132,7 +8133,7 @@
         <v>5.5981880994604438E-3</v>
       </c>
     </row>
-    <row r="238" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="14" t="s">
         <v>294</v>
       </c>
@@ -8146,7 +8147,7 @@
         <v>7.87093476212707</v>
       </c>
     </row>
-    <row r="239" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="14" t="s">
         <v>295</v>
       </c>
@@ -8192,7 +8193,7 @@
         <v>5.392089089202301E-4</v>
       </c>
     </row>
-    <row r="240" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="14" t="s">
         <v>296</v>
       </c>
@@ -8206,7 +8207,7 @@
         <v>7.8838242011011399</v>
       </c>
     </row>
-    <row r="241" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="14" t="s">
         <v>297</v>
       </c>
@@ -8220,7 +8221,7 @@
         <v>8.1335197047369494</v>
       </c>
     </row>
-    <row r="242" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="14" t="s">
         <v>298</v>
       </c>
@@ -8266,7 +8267,7 @@
         <v>3.062021826470307E-3</v>
       </c>
     </row>
-    <row r="243" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="14" t="s">
         <v>299</v>
       </c>
@@ -8280,7 +8281,7 @@
         <v>7.715093927551</v>
       </c>
     </row>
-    <row r="244" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="14" t="s">
         <v>300</v>
       </c>
@@ -8294,7 +8295,7 @@
         <v>7.71823273259385</v>
       </c>
     </row>
-    <row r="245" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="14" t="s">
         <v>301</v>
       </c>
@@ -8308,7 +8309,7 @@
         <v>7.7164851704236099</v>
       </c>
     </row>
-    <row r="246" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="14" t="s">
         <v>302</v>
       </c>
@@ -8322,7 +8323,7 @@
         <v>7.7176880414598603</v>
       </c>
     </row>
-    <row r="247" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="14" t="s">
         <v>303</v>
       </c>
@@ -8336,7 +8337,7 @@
         <v>7.7176845907370097</v>
       </c>
     </row>
-    <row r="248" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="14" t="s">
         <v>304</v>
       </c>
@@ -8350,7 +8351,7 @@
         <v>7.7177699275983898</v>
       </c>
     </row>
-    <row r="249" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="14" t="s">
         <v>305</v>
       </c>
@@ -8364,8 +8365,8 @@
         <v>7.8915308513717601</v>
       </c>
       <c r="G249" s="15">
-        <f>AVERAGE(D249:D250)</f>
-        <v>7.9651952085418198</v>
+        <f>AVERAGE(D249:D251)</f>
+        <v>7.9643186141655136</v>
       </c>
       <c r="H249" s="14">
         <f>_xlfn.STDEV.S(D249:D250)</f>
@@ -8377,11 +8378,11 @@
       </c>
       <c r="J249" s="14">
         <f>H249/G249</f>
-        <v>4.2400193706731388E-5</v>
+        <v>4.2404860492825495E-5</v>
       </c>
       <c r="K249" s="19">
         <f>J249</f>
-        <v>4.2400193706731388E-5</v>
+        <v>4.2404860492825495E-5</v>
       </c>
       <c r="L249" s="15">
         <f>MIN(D249:D250)</f>
@@ -8396,7 +8397,7 @@
         <v>4.7761643465982218E-4</v>
       </c>
     </row>
-    <row r="250" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="14" t="s">
         <v>306</v>
       </c>
@@ -8410,7 +8411,7 @@
         <v>7.8910532349370897</v>
       </c>
     </row>
-    <row r="251" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="14" t="s">
         <v>307</v>
       </c>
@@ -8424,7 +8425,7 @@
         <v>7.8886622600254999</v>
       </c>
     </row>
-    <row r="252" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="14" t="s">
         <v>308</v>
       </c>
@@ -8438,8 +8439,8 @@
         <v>7.8265004448522104</v>
       </c>
       <c r="G252" s="15">
-        <f>AVERAGE(D252:D253)</f>
-        <v>7.9496252425503258</v>
+        <f>AVERAGE(D252:D254)</f>
+        <v>7.9492016477328109</v>
       </c>
       <c r="H252" s="14">
         <f>_xlfn.STDEV.S(D252:D253)</f>
@@ -8451,11 +8452,11 @@
       </c>
       <c r="J252" s="14">
         <f>H252/G252</f>
-        <v>1.7238059174729635E-4</v>
+        <v>1.7238977751569677E-4</v>
       </c>
       <c r="K252" s="19">
         <f>J252</f>
-        <v>1.7238059174729635E-4</v>
+        <v>1.7238977751569677E-4</v>
       </c>
       <c r="L252" s="15">
         <f>MIN(D252:D253)</f>
@@ -8470,7 +8471,7 @@
         <v>1.9379832578900746E-3</v>
       </c>
     </row>
-    <row r="253" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="14" t="s">
         <v>309</v>
       </c>
@@ -8484,7 +8485,7 @@
         <v>7.8245624615943301</v>
       </c>
     </row>
-    <row r="254" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="14" t="s">
         <v>310</v>
       </c>
@@ -8498,7 +8499,7 @@
         <v>7.8242606687707301</v>
       </c>
     </row>
-    <row r="255" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="14" t="s">
         <v>311</v>
       </c>
@@ -8512,8 +8513,8 @@
         <v>7.7878980637266499</v>
       </c>
       <c r="G255" s="15">
-        <f>AVERAGE(D255:D256)</f>
-        <v>7.9269637838006002</v>
+        <f>AVERAGE(D255:D257)</f>
+        <v>7.9256810439087433</v>
       </c>
       <c r="H255" s="14">
         <f>_xlfn.STDEV.S(D255:D256)</f>
@@ -8525,11 +8526,11 @@
       </c>
       <c r="J255" s="14">
         <f>H255/G255</f>
-        <v>1.3869769806390729E-4</v>
+        <v>1.3872014573360655E-4</v>
       </c>
       <c r="K255" s="19">
         <f>J255</f>
-        <v>1.3869769806390729E-4</v>
+        <v>1.3872014573360655E-4</v>
       </c>
       <c r="L255" s="15">
         <f>MIN(D255:D256)</f>
@@ -8544,7 +8545,7 @@
         <v>1.554859405540121E-3</v>
       </c>
     </row>
-    <row r="256" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="14" t="s">
         <v>312</v>
       </c>
@@ -8558,7 +8559,7 @@
         <v>7.7863432043211098</v>
       </c>
     </row>
-    <row r="257" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="14" t="s">
         <v>313</v>
       </c>
@@ -8573,8 +8574,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O191"/>
-  <sortState ref="A2:O144">
+  <autoFilter ref="A1:O191" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O144">
     <sortCondition ref="B2:B144"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8583,7 +8584,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
@@ -8591,25 +8592,25 @@
       <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="103" style="6" customWidth="1"/>
-    <col min="11" max="11" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.5546875" style="9" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.88671875" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.5703125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>40</v>
       </c>
@@ -8643,7 +8644,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>53</v>
       </c>
@@ -8680,7 +8681,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>61</v>
       </c>
@@ -8707,7 +8708,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>77</v>
       </c>
@@ -8737,7 +8738,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>95</v>
       </c>
@@ -8770,7 +8771,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>98</v>
       </c>
@@ -8800,7 +8801,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>102</v>
       </c>
@@ -8820,7 +8821,7 @@
         <v>1.4675794477244731E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>130</v>
       </c>
@@ -8840,7 +8841,7 @@
         <v>9.5489994253788926E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>112</v>
       </c>
@@ -8860,7 +8861,7 @@
         <v>1.516738390249465E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>197</v>
       </c>
@@ -8880,7 +8881,7 @@
         <v>3.5994366965510827E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>297</v>
       </c>
@@ -8900,42 +8901,42 @@
         <v>1.5976496949771635E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="25"/>
       <c r="C12" s="26"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
       <c r="B13" s="25"/>
       <c r="C13" s="26"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="25"/>
       <c r="C14" s="26"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
       <c r="B15" s="25"/>
       <c r="C15" s="26"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="25"/>
       <c r="C16" s="26"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="25"/>
       <c r="C17" s="26"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="25"/>
       <c r="C18" s="26"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
       <c r="B19" s="25"/>
       <c r="C19" s="26"/>
@@ -8946,7 +8947,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="B20" s="25"/>
       <c r="C20" s="26"/>
@@ -8957,147 +8958,147 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="24"/>
       <c r="B21" s="25"/>
       <c r="C21" s="26"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="24"/>
       <c r="B22" s="25"/>
       <c r="C22" s="26"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="24"/>
       <c r="B23" s="25"/>
       <c r="C23" s="26"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="24"/>
       <c r="B24" s="25"/>
       <c r="C24" s="26"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
       <c r="B25" s="25"/>
       <c r="C25" s="26"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C26" s="26"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C27" s="26"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C28" s="26"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C29" s="26"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C30" s="26"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C31" s="26"/>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C32" s="26"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="26"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="26"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="26"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" s="26"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="26"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" s="26"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" s="26"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" s="26"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="26"/>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" s="26"/>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" s="26"/>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" s="26"/>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" s="26"/>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46" s="26"/>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="26"/>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" s="26"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="26"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="26"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="26"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="26"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="26"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="26"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="26"/>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="26"/>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="26"/>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" s="26"/>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="26"/>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" s="26"/>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="26"/>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" s="26"/>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" s="26"/>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" s="26"/>
     </row>
   </sheetData>
@@ -9108,32 +9109,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="103" style="6" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" style="9" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="10" customWidth="1"/>
-    <col min="14" max="14" width="20.109375" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="9" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="10" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -9164,7 +9165,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>153</v>
       </c>
@@ -9205,7 +9206,7 @@
         <v>11.92</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>160</v>
       </c>
@@ -9234,7 +9235,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>171</v>
       </c>
@@ -9264,7 +9265,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>177</v>
       </c>
@@ -9294,7 +9295,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>187</v>
       </c>
@@ -9314,7 +9315,7 @@
         <v>6.0364966713408619E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>239</v>
       </c>
@@ -9334,7 +9335,7 @@
         <v>1.3899760750579057E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>240</v>
       </c>
@@ -9354,7 +9355,7 @@
         <v>9.5872032397609086E-7</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>204</v>
       </c>
@@ -9374,7 +9375,7 @@
         <v>2.2764778095089857E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>205</v>
       </c>
@@ -9394,7 +9395,7 @@
         <v>2.5736318323859534E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>225</v>
       </c>
@@ -9414,7 +9415,7 @@
         <v>3.6664135788884965E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>224</v>
       </c>
@@ -9434,37 +9435,37 @@
         <v>3.1966359315675798E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
@@ -9475,7 +9476,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C20" s="9"/>
       <c r="F20" s="7" t="s">
         <v>38</v>
@@ -9484,22 +9485,22 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C22" s="9"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C23" s="9"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C24" s="9"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C25" s="9"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F31" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the most recent round of pH data to the QAQC file. Found that min and max in the excel file had been calculated incorrectly anywhere there were more than two replicates. An easy fix once I found out that was happening.
I updated the Bay Standards sheet to have the new environmental data from the Bay Standard Batch 2 that I made.

The most recent bay standard and Dickson TRIS Seawater buffer run looked solid and we should be good moving forward with the new bay standard batch.
</commit_message>
<xml_diff>
--- a/check sample work/pH QAQC/20210326 pH check sample results summary.xlsx
+++ b/check sample work/pH QAQC/20210326 pH check sample results summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rye-Tech\Documents\R\rye-tech-home\2021-season-summary\check sample work\pH QAQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A54FF7-D474-46A3-85FE-6DC4DD0F7A8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6152E834-7FA6-4BBA-ABCF-981BC9497B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="334">
   <si>
     <t>sample</t>
   </si>
@@ -759,9 +759,6 @@
     <t>Bay STD</t>
   </si>
   <si>
-    <t>First Sample</t>
-  </si>
-  <si>
     <t xml:space="preserve"> https://sfsu.box.com/s/e9d5xj7c425bnurrwe2x98ky57q5hh8e </t>
   </si>
   <si>
@@ -973,6 +970,69 @@
   </si>
   <si>
     <t xml:space="preserve"> P-0034-C1-P3-E</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BAYSTD1-07APR2021-D</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P-0084-C1-R1-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P-0084-C1-R2-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P-0084-C1-R5-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P-0084-C1-R6-B</t>
+  </si>
+  <si>
+    <t>scattered test day for Byron and Chelsey</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DIC-CRM186-1-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DIC-CRM186-2-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DIC-CRM186-3-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BAYSTD1-1-B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BAYSTD1-2-D</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BAYSTD1-3-E</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BAYSTD2-1-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BAYSTD2-2-G</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BAYSTD2-3-4</t>
+  </si>
+  <si>
+    <t>Sample was murky with sediment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BAYSTD1-04272021</t>
+  </si>
+  <si>
+    <t>DIC-04-27-2021</t>
+  </si>
+  <si>
+    <t>Bay Std Batch 1</t>
+  </si>
+  <si>
+    <t>Batch 1</t>
+  </si>
+  <si>
+    <t>Batch 2</t>
   </si>
 </sst>
 </file>
@@ -1041,7 +1101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1105,6 +1165,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2182,11 +2245,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O257"/>
+  <dimension ref="A1:O271"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G255" activeCellId="2" sqref="G249 G252 G255"/>
+      <pane ySplit="1" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A263" sqref="A263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2379,16 +2442,16 @@
         <v>7.2824193958023731E-4</v>
       </c>
       <c r="L6" s="15">
-        <f>MIN(D6:D7)</f>
-        <v>7.9789145799999996</v>
+        <f>MIN(D6:D11)</f>
+        <v>7.9724865879999998</v>
       </c>
       <c r="M6" s="15">
-        <f>MAX(D6:D7)</f>
+        <f>MAX(D6:D11)</f>
         <v>7.9888786669999998</v>
       </c>
       <c r="N6" s="14">
         <f>M6-L6</f>
-        <v>9.9640870000001769E-3</v>
+        <v>1.6392079000000059E-2</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2539,16 +2602,16 @@
         <v>8.7124200150286515E-4</v>
       </c>
       <c r="L13" s="15">
-        <f>MIN(D13:D14)</f>
+        <f>MIN(D13:D15)</f>
         <v>7.9771397199617002</v>
       </c>
       <c r="M13" s="15">
-        <f>MAX(D13:D14)</f>
-        <v>7.9831010909762803</v>
+        <f>MAX(D13:D15)</f>
+        <v>7.9910059490455501</v>
       </c>
       <c r="N13" s="14">
         <f>M13-L13</f>
-        <v>5.9613710145800525E-3</v>
+        <v>1.3866229083849824E-2</v>
       </c>
       <c r="O13" s="20"/>
     </row>
@@ -2716,16 +2779,16 @@
         <v>4.0826381491328395E-4</v>
       </c>
       <c r="L22" s="15">
-        <f>MIN(D22:D23)</f>
-        <v>7.9557810703072001</v>
+        <f>MIN(D22:D24)</f>
+        <v>7.9553757482688896</v>
       </c>
       <c r="M22" s="15">
-        <f>MAX(D22:D23)</f>
+        <f>MAX(D22:D24)</f>
         <v>7.9611944311944303</v>
       </c>
       <c r="N22" s="14">
         <f>M22-L22</f>
-        <v>5.4133608872302119E-3</v>
+        <v>5.8186829255406636E-3</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2790,16 +2853,16 @@
         <v>5.3561856706451911E-4</v>
       </c>
       <c r="L25" s="15">
-        <f>MIN(D25:D26)</f>
+        <f>MIN(D25:D27)</f>
         <v>7.9812642389606001</v>
       </c>
       <c r="M25" s="15">
-        <f>MAX(D25:D26)</f>
-        <v>7.9843874831025499</v>
+        <f>MAX(D25:D27)</f>
+        <v>7.98972236087869</v>
       </c>
       <c r="N25" s="14">
         <f>M25-L25</f>
-        <v>3.1232441419497547E-3</v>
+        <v>8.4581219180899225E-3</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2878,16 +2941,16 @@
         <v>8.8765772194442961E-4</v>
       </c>
       <c r="L29" s="15">
-        <f>MIN(D29:D30)</f>
+        <f>MIN(D29:D31)</f>
         <v>8.1607421721078293</v>
       </c>
       <c r="M29" s="15">
-        <f>MAX(D29:D30)</f>
-        <v>8.1714628035159809</v>
+        <f>MAX(D29:D31)</f>
+        <v>8.1745606813405001</v>
       </c>
       <c r="N29" s="14">
         <f>M29-L29</f>
-        <v>1.0720631408151604E-2</v>
+        <v>1.3818509232670806E-2</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2952,11 +3015,11 @@
         <v>1.4007622871273979E-3</v>
       </c>
       <c r="L32" s="15">
-        <f>MIN(D32:D33)</f>
+        <f>MIN(D32:D34)</f>
         <v>7.9494502463219598</v>
       </c>
       <c r="M32" s="15">
-        <f>MAX(D32:D33)</f>
+        <f>MAX(D32:D34)</f>
         <v>7.9717148226389396</v>
       </c>
       <c r="N32" s="14">
@@ -3027,16 +3090,16 @@
         <v>3.6391442455792791E-3</v>
       </c>
       <c r="L35" s="15">
-        <f>MIN(D35:D36)</f>
-        <v>7.749798792</v>
+        <f>MIN(D35:D37)</f>
+        <v>7.7022063860000003</v>
       </c>
       <c r="M35" s="15">
-        <f>MAX(D35:D36)</f>
+        <f>MAX(D35:D37)</f>
         <v>7.7520427249999999</v>
       </c>
       <c r="N35" s="14">
         <f>M35-L35</f>
-        <v>2.2439329999999202E-3</v>
+        <v>4.9836338999999619E-2</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3109,11 +3172,11 @@
         <v>7.098771892717616E-4</v>
       </c>
       <c r="L38" s="15">
-        <f>MIN(D38:D39)</f>
+        <f>MIN(D38:D40)</f>
         <v>7.83028325429615</v>
       </c>
       <c r="M38" s="15">
-        <f>MAX(D38:D39)</f>
+        <f>MAX(D38:D40)</f>
         <v>7.8404368469605803</v>
       </c>
       <c r="N38" s="14">
@@ -3183,16 +3246,16 @@
         <v>3.6279295946290663E-3</v>
       </c>
       <c r="L41" s="15">
-        <f>MIN(D41:D42)</f>
-        <v>7.7498648020787897</v>
+        <f>MIN(D41:D43)</f>
+        <v>7.7024167596355504</v>
       </c>
       <c r="M41" s="15">
-        <f>MAX(D41:D42)</f>
+        <f>MAX(D41:D43)</f>
         <v>7.7520988197778298</v>
       </c>
       <c r="N41" s="14">
         <f>M41-L41</f>
-        <v>2.2340176990400806E-3</v>
+        <v>4.9682060142279383E-2</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3257,16 +3320,16 @@
         <v>4.4256429010785012E-4</v>
       </c>
       <c r="L44" s="15">
-        <f>MIN(D44:D45)</f>
-        <v>7.8410398633777296</v>
+        <f>MIN(D44:D46)</f>
+        <v>7.8400472210670502</v>
       </c>
       <c r="M44" s="15">
-        <f>MAX(D44:D45)</f>
+        <f>MAX(D44:D46)</f>
         <v>7.8464934009292699</v>
       </c>
       <c r="N44" s="14">
         <f>M44-L44</f>
-        <v>5.4535375515403217E-3</v>
+        <v>6.4461798622197364E-3</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3331,16 +3394,16 @@
         <v>1.4199776864768217E-4</v>
       </c>
       <c r="L47" s="15">
-        <f>MIN(D47:D48)</f>
-        <v>7.9944032779947802</v>
+        <f>MIN(D47:D49)</f>
+        <v>7.9943636123524699</v>
       </c>
       <c r="M47" s="15">
-        <f>MAX(D47:D48)</f>
+        <f>MAX(D47:D49)</f>
         <v>7.9963495037024304</v>
       </c>
       <c r="N47" s="14">
         <f>M47-L47</f>
-        <v>1.9462257076501288E-3</v>
+        <v>1.9858913499604114E-3</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3489,16 +3552,16 @@
         <v>1.3634419026510095E-4</v>
       </c>
       <c r="L56" s="15">
-        <f>MIN(D56:D57)</f>
-        <v>8.0033502253286795</v>
+        <f>MIN(D56:D58)</f>
+        <v>8.0015489896471905</v>
       </c>
       <c r="M56" s="15">
-        <f>MAX(D56:D57)</f>
+        <f>MAX(D56:D58)</f>
         <v>8.0035165638346193</v>
       </c>
       <c r="N56" s="14">
         <f>M56-L56</f>
-        <v>1.6633850593983368E-4</v>
+        <v>1.9675741874287667E-3</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3555,6 +3618,9 @@
       </c>
       <c r="E60" s="15">
         <v>7.1785394059999996</v>
+      </c>
+      <c r="F60" s="16" t="s">
+        <v>318</v>
       </c>
       <c r="G60" s="15"/>
       <c r="K60" s="19"/>
@@ -3574,6 +3640,9 @@
       <c r="E61" s="15">
         <v>7.1826006600000003</v>
       </c>
+      <c r="F61" s="16" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="62" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
@@ -3588,6 +3657,9 @@
       <c r="E62" s="15">
         <v>7.2032755269999997</v>
       </c>
+      <c r="F62" s="16" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="63" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
@@ -3602,6 +3674,9 @@
       <c r="E63" s="15">
         <v>7.7168752789999999</v>
       </c>
+      <c r="F63" s="16" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="64" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
@@ -3616,6 +3691,9 @@
       <c r="E64" s="15">
         <v>6.0824875330000001</v>
       </c>
+      <c r="F64" s="16" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="65" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
@@ -3630,6 +3708,9 @@
       <c r="E65" s="15">
         <v>7.7928240129999997</v>
       </c>
+      <c r="F65" s="16" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="66" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
@@ -3644,6 +3725,9 @@
       <c r="E66" s="15">
         <v>7.1200401400000004</v>
       </c>
+      <c r="F66" s="16" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="67" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
@@ -3658,6 +3742,9 @@
       <c r="E67" s="15">
         <v>7.6971565870000003</v>
       </c>
+      <c r="F67" s="16" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="68" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
@@ -3672,6 +3759,9 @@
       <c r="E68" s="15">
         <v>7.1042788000000003</v>
       </c>
+      <c r="F68" s="16" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="69" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
@@ -3707,16 +3797,16 @@
         <v>2.0451023310936027E-4</v>
       </c>
       <c r="L69" s="15">
-        <f>MIN(D69:D70)</f>
-        <v>7.8865123080000004</v>
+        <f>MIN(D69:D72)</f>
+        <v>7.8849200000000002</v>
       </c>
       <c r="M69" s="15">
-        <f>MAX(D69:D70)</f>
-        <v>7.8869022700000002</v>
+        <f>MAX(D69:D72)</f>
+        <v>7.8888438010000002</v>
       </c>
       <c r="N69" s="14">
         <f>M69-L69</f>
-        <v>3.8996199999985492E-4</v>
+        <v>3.9238010000000045E-3</v>
       </c>
     </row>
     <row r="70" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3795,16 +3885,16 @@
         <v>1.2292781717221677E-2</v>
       </c>
       <c r="L73" s="15">
-        <f>MIN(D73:D74)</f>
-        <v>7.2212618180000003</v>
+        <f>MIN(D73:D75)</f>
+        <v>7.2005980059999999</v>
       </c>
       <c r="M73" s="15">
-        <f>MAX(D73:D74)</f>
+        <f>MAX(D73:D75)</f>
         <v>7.3645139970000004</v>
       </c>
       <c r="N73" s="14">
         <f>M73-L73</f>
-        <v>0.14325217900000009</v>
+        <v>0.16391599100000054</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3883,16 +3973,16 @@
         <v>1.3602336509237246E-3</v>
       </c>
       <c r="L77" s="15">
-        <f>MIN(D77:D78)</f>
-        <v>7.3913682520000004</v>
+        <f>MIN(D77:D79)</f>
+        <v>7.3784985409999999</v>
       </c>
       <c r="M77" s="15">
-        <f>MAX(D77:D78)</f>
+        <f>MAX(D77:D79)</f>
         <v>7.3983073910000003</v>
       </c>
       <c r="N77" s="14">
         <f>M77-L77</f>
-        <v>6.9391389999999831E-3</v>
+        <v>1.9808850000000433E-2</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3957,16 +4047,16 @@
         <v>3.344306410987987E-4</v>
       </c>
       <c r="L80" s="15">
-        <f>MIN(D80:D81)</f>
-        <v>7.9175234410000002</v>
+        <f>MIN(D80:D82)</f>
+        <v>7.9153278919999996</v>
       </c>
       <c r="M80" s="15">
-        <f>MAX(D80:D81)</f>
+        <f>MAX(D80:D82)</f>
         <v>7.9205993650000002</v>
       </c>
       <c r="N80" s="14">
         <f>M80-L80</f>
-        <v>3.0759240000000077E-3</v>
+        <v>5.2714730000005261E-3</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4271,16 +4361,16 @@
         <v>7.2186079493474829E-4</v>
       </c>
       <c r="L91" s="15">
-        <f>MIN(D91:D92)</f>
-        <v>7.9557416139999999</v>
+        <f>MIN(D91:D93)</f>
+        <v>7.9465864860000002</v>
       </c>
       <c r="M91" s="15">
-        <f>MAX(D91:D92)</f>
+        <f>MAX(D91:D93)</f>
         <v>7.9571655200000002</v>
       </c>
       <c r="N91" s="14">
         <f>M91-L91</f>
-        <v>1.4239060000003079E-3</v>
+        <v>1.0579034000000043E-2</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4345,16 +4435,16 @@
         <v>6.6642328682573805E-4</v>
       </c>
       <c r="L94" s="15">
-        <f>MIN(D94:D95)</f>
+        <f>MIN(D94:D96)</f>
         <v>7.9512931179999997</v>
       </c>
       <c r="M94" s="15">
-        <f>MAX(D94:D95)</f>
-        <v>7.9534403789999999</v>
+        <f>MAX(D94:D96)</f>
+        <v>7.9613591960000001</v>
       </c>
       <c r="N94" s="14">
         <f>M94-L94</f>
-        <v>2.1472610000001779E-3</v>
+        <v>1.0066078000000367E-2</v>
       </c>
     </row>
     <row r="95" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4419,16 +4509,16 @@
         <v>1.0702146173680953E-3</v>
       </c>
       <c r="L97" s="15">
-        <f>MIN(D97:D98)</f>
+        <f>MIN(D97:D99)</f>
         <v>7.9205601489999999</v>
       </c>
       <c r="M97" s="15">
-        <f>MAX(D97:D98)</f>
-        <v>7.9231002330000004</v>
+        <f>MAX(D97:D99)</f>
+        <v>7.9363579959999999</v>
       </c>
       <c r="N97" s="14">
         <f>M97-L97</f>
-        <v>2.5400840000004976E-3</v>
+        <v>1.5797846999999976E-2</v>
       </c>
     </row>
     <row r="98" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4493,16 +4583,16 @@
         <v>4.9755139347742864E-4</v>
       </c>
       <c r="L100" s="15">
-        <f>MIN(D100:D101)</f>
-        <v>7.9397894820000001</v>
+        <f>MIN(D100:D102)</f>
+        <v>7.9366448979999999</v>
       </c>
       <c r="M100" s="15">
-        <f>MAX(D100:D101)</f>
+        <f>MAX(D100:D102)</f>
         <v>7.9444947749999999</v>
       </c>
       <c r="N100" s="14">
         <f>M100-L100</f>
-        <v>4.7052929999997772E-3</v>
+        <v>7.8498769999999496E-3</v>
       </c>
     </row>
     <row r="101" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4585,11 +4675,11 @@
         <v>5.5034875675458172E-4</v>
       </c>
       <c r="L104" s="15">
-        <f>MIN(D104:D105)</f>
+        <f>MIN(D104:D106)</f>
         <v>7.8241510209999996</v>
       </c>
       <c r="M104" s="15">
-        <f>MAX(D104:D105)</f>
+        <f>MAX(D104:D106)</f>
         <v>7.8327470200000002</v>
       </c>
       <c r="N104" s="14">
@@ -4659,16 +4749,16 @@
         <v>1.5794662718664388E-4</v>
       </c>
       <c r="L107" s="15">
-        <f>MIN(D107:D108)</f>
-        <v>7.8035179259999996</v>
+        <f>MIN(D107:D109)</f>
+        <v>7.8018158099999999</v>
       </c>
       <c r="M107" s="15">
-        <f>MAX(D107:D108)</f>
+        <f>MAX(D107:D109)</f>
         <v>7.8042109430000002</v>
       </c>
       <c r="N107" s="14">
         <f>M107-L107</f>
-        <v>6.9301700000057309E-4</v>
+        <v>2.3951330000002713E-3</v>
       </c>
     </row>
     <row r="108" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4747,16 +4837,16 @@
         <v>4.6391331890809512E-4</v>
       </c>
       <c r="L111" s="15">
-        <f>MIN(D111:D112)</f>
+        <f>MIN(D111:D113)</f>
         <v>7.3095219609999997</v>
       </c>
       <c r="M111" s="15">
-        <f>MAX(D111:D112)</f>
-        <v>7.310091495</v>
+        <f>MAX(D111:D113)</f>
+        <v>7.3156611419999997</v>
       </c>
       <c r="N111" s="14">
         <f>M111-L111</f>
-        <v>5.6953400000026022E-4</v>
+        <v>6.1391809999999936E-3</v>
       </c>
     </row>
     <row r="112" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4821,16 +4911,16 @@
         <v>3.0990325776475474E-4</v>
       </c>
       <c r="L114" s="15">
-        <f>MIN(D114:D115)</f>
+        <f>MIN(D114:D116)</f>
         <v>7.633827814</v>
       </c>
       <c r="M114" s="15">
-        <f>MAX(D114:D115)</f>
-        <v>7.6377435279999997</v>
+        <f>MAX(D114:D116)</f>
+        <v>7.6380884240000002</v>
       </c>
       <c r="N114" s="14">
         <f>M114-L114</f>
-        <v>3.9157139999996815E-3</v>
+        <v>4.2606100000002201E-3</v>
       </c>
     </row>
     <row r="115" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4909,11 +4999,11 @@
         <v>2.9835195347258536E-5</v>
       </c>
       <c r="L118" s="15">
-        <f>MIN(D118:D119)</f>
+        <f>MIN(D118:D120)</f>
         <v>7.8373963010000001</v>
       </c>
       <c r="M118" s="15">
-        <f>MAX(D118:D119)</f>
+        <f>MAX(D118:D120)</f>
         <v>7.8378624940000003</v>
       </c>
       <c r="N118" s="14">
@@ -4983,11 +5073,11 @@
         <v>2.3422230178035298E-4</v>
       </c>
       <c r="L121" s="15">
-        <f>MIN(D121:D122)</f>
+        <f>MIN(D121:D123)</f>
         <v>7.8028915110000003</v>
       </c>
       <c r="M121" s="15">
-        <f>MAX(D121:D122)</f>
+        <f>MAX(D121:D123)</f>
         <v>7.8061551119999999</v>
       </c>
       <c r="N121" s="14">
@@ -5057,11 +5147,11 @@
         <v>8.039867020416901E-4</v>
       </c>
       <c r="L124" s="15">
-        <f>MIN(D124:D125)</f>
+        <f>MIN(D124:D126)</f>
         <v>6.5294750800000001</v>
       </c>
       <c r="M124" s="15">
-        <f>MAX(D124:D125)</f>
+        <f>MAX(D124:D126)</f>
         <v>6.5393071149999997</v>
       </c>
       <c r="N124" s="14">
@@ -5160,16 +5250,16 @@
         <v>1.3240741263768291E-4</v>
       </c>
       <c r="L129" s="15">
-        <f>MIN(D129:D130)</f>
+        <f>MIN(D129:D131)</f>
         <v>7.8218839109999996</v>
       </c>
       <c r="M129" s="15">
-        <f>MAX(D129:D130)</f>
-        <v>7.8236250299999996</v>
+        <f>MAX(D129:D131)</f>
+        <v>7.823726701</v>
       </c>
       <c r="N129" s="14">
         <f>M129-L129</f>
-        <v>1.7411190000000687E-3</v>
+        <v>1.8427900000004271E-3</v>
       </c>
     </row>
     <row r="130" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -5276,11 +5366,11 @@
         <v>7.3235681856344606E-4</v>
       </c>
       <c r="L135" s="15">
-        <f>MIN(D135:D136)</f>
+        <f>MIN(D135:D137)</f>
         <v>7.8314022960000003</v>
       </c>
       <c r="M135" s="15">
-        <f>MAX(D135:D136)</f>
+        <f>MAX(D135:D137)</f>
         <v>7.8428811769999998</v>
       </c>
       <c r="N135" s="14">
@@ -5350,16 +5440,16 @@
         <v>5.3071718186280053E-4</v>
       </c>
       <c r="L138" s="15">
-        <f>MIN(D138:D139)</f>
-        <v>7.8532079179999998</v>
+        <f>MIN(D138:D140)</f>
+        <v>7.8498468499999996</v>
       </c>
       <c r="M138" s="15">
-        <f>MAX(D138:D139)</f>
+        <f>MAX(D138:D140)</f>
         <v>7.8581339579999998</v>
       </c>
       <c r="N138" s="14">
         <f>M138-L138</f>
-        <v>4.9260399999999649E-3</v>
+        <v>8.2871080000002095E-3</v>
       </c>
     </row>
     <row r="139" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -5424,16 +5514,16 @@
         <v>8.4988883330988098E-4</v>
       </c>
       <c r="L141" s="15">
-        <f>MIN(D141:D142)</f>
+        <f>MIN(D141:D143)</f>
         <v>7.8466364610000001</v>
       </c>
       <c r="M141" s="15">
-        <f>MAX(D141:D142)</f>
-        <v>7.8492889039999998</v>
+        <f>MAX(D141:D143)</f>
+        <v>7.8592902770000004</v>
       </c>
       <c r="N141" s="14">
         <f>M141-L141</f>
-        <v>2.6524429999996713E-3</v>
+        <v>1.2653816000000262E-2</v>
       </c>
     </row>
     <row r="142" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -5515,16 +5605,16 @@
         <v>2.2638662478616418E-4</v>
       </c>
       <c r="L145" s="15">
-        <f>MIN(D145:D146)</f>
+        <f>MIN(D145:D147)</f>
         <v>8.0621109035941299</v>
       </c>
       <c r="M145" s="15">
-        <f>MAX(D145:D146)</f>
-        <v>8.0628483060290908</v>
+        <f>MAX(D145:D147)</f>
+        <v>8.0655762503862594</v>
       </c>
       <c r="N145" s="14">
         <f>M145-L145</f>
-        <v>7.3740243496089874E-4</v>
+        <v>3.4653467921295089E-3</v>
       </c>
     </row>
     <row r="146" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -5598,11 +5688,11 @@
         <v>4.0415549261917756E-4</v>
       </c>
       <c r="L148" s="15">
-        <f>MIN(D148:D149)</f>
+        <f>MIN(D148:D150)</f>
         <v>8.0629114271487694</v>
       </c>
       <c r="M148" s="15">
-        <f>MAX(D148:D149)</f>
+        <f>MAX(D148:D150)</f>
         <v>8.0688796541484091</v>
       </c>
       <c r="N148" s="14">
@@ -5681,11 +5771,11 @@
         <v>6.1007972935448926E-4</v>
       </c>
       <c r="L151" s="15">
-        <f>MIN(D151:D152)</f>
+        <f>MIN(D151:D153)</f>
         <v>8.1111947586784705</v>
       </c>
       <c r="M151" s="15">
-        <f>MAX(D151:D152)</f>
+        <f>MAX(D151:D153)</f>
         <v>8.1209519099859602</v>
       </c>
       <c r="N151" s="14">
@@ -5798,16 +5888,16 @@
         <v>2.8764408012332446E-4</v>
       </c>
       <c r="L156" s="15">
-        <f>MIN(D156:D157)</f>
+        <f>MIN(D156:D158)</f>
         <v>7.7590701304939298</v>
       </c>
       <c r="M156" s="15">
-        <f>MAX(D156:D157)</f>
-        <v>7.7611215224821501</v>
+        <f>MAX(D156:D158)</f>
+        <v>7.7635303098703998</v>
       </c>
       <c r="N156" s="14">
         <f>M156-L156</f>
-        <v>2.0513919882203524E-3</v>
+        <v>4.4601793764700304E-3</v>
       </c>
     </row>
     <row r="157" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -5898,16 +5988,16 @@
         <v>1.8715843105971373E-4</v>
       </c>
       <c r="L160" s="15">
-        <f>MIN(D160:D161)</f>
+        <f>MIN(D160:D162)</f>
         <v>7.7695701272574302</v>
       </c>
       <c r="M160" s="15">
-        <f>MAX(D160:D161)</f>
-        <v>7.7719698752695798</v>
+        <f>MAX(D160:D162)</f>
+        <v>7.7721938046073298</v>
       </c>
       <c r="N160" s="14">
         <f>M160-L160</f>
-        <v>2.399748012149594E-3</v>
+        <v>2.6236773498995447E-3</v>
       </c>
     </row>
     <row r="161" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6436,7 +6526,7 @@
         <v>7.85323673583241</v>
       </c>
       <c r="F180" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G180" s="15">
         <f>AVERAGE(D180:D182)</f>
@@ -6459,16 +6549,16 @@
         <v>8.727245236408724E-3</v>
       </c>
       <c r="L180" s="15">
-        <f>MIN(D180:D181)</f>
+        <f>MIN(D180:D182)</f>
         <v>7.9253754091890798</v>
       </c>
       <c r="M180" s="15">
-        <f>MAX(D180:D181)</f>
-        <v>7.9785195004651799</v>
+        <f>MAX(D180:D182)</f>
+        <v>8.0635979587047792</v>
       </c>
       <c r="N180" s="14">
         <f>M180-L180</f>
-        <v>5.3144091276100092E-2</v>
+        <v>0.13822254951569946</v>
       </c>
     </row>
     <row r="181" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6485,7 +6575,7 @@
         <v>7.8000926445563001</v>
       </c>
       <c r="F181" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="182" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6502,7 +6592,7 @@
         <v>7.9383151940719996</v>
       </c>
       <c r="F182" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="183" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6779,7 +6869,7 @@
     </row>
     <row r="193" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B193" s="18">
         <v>44131</v>
@@ -6825,7 +6915,7 @@
     </row>
     <row r="194" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B194" s="18">
         <v>44131</v>
@@ -6839,7 +6929,7 @@
     </row>
     <row r="195" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B195" s="18">
         <v>44131</v>
@@ -6885,7 +6975,7 @@
     </row>
     <row r="196" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B196" s="18">
         <v>44131</v>
@@ -6899,7 +6989,7 @@
     </row>
     <row r="197" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B197" s="18">
         <v>44131</v>
@@ -6945,7 +7035,7 @@
     </row>
     <row r="198" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B198" s="18">
         <v>44131</v>
@@ -6959,7 +7049,7 @@
     </row>
     <row r="199" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B199" s="18">
         <v>44131</v>
@@ -7005,7 +7095,7 @@
     </row>
     <row r="200" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B200" s="18">
         <v>44131</v>
@@ -7019,7 +7109,7 @@
     </row>
     <row r="201" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B201" s="18">
         <v>44131</v>
@@ -7033,7 +7123,7 @@
     </row>
     <row r="202" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B202" s="18">
         <v>44131</v>
@@ -7079,7 +7169,7 @@
     </row>
     <row r="203" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B203" s="18">
         <v>44131</v>
@@ -7093,7 +7183,7 @@
     </row>
     <row r="204" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B204" s="18">
         <v>44131</v>
@@ -7139,7 +7229,7 @@
     </row>
     <row r="205" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B205" s="18">
         <v>44131</v>
@@ -7153,7 +7243,7 @@
     </row>
     <row r="206" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B206" s="18">
         <v>44131</v>
@@ -7199,7 +7289,7 @@
     </row>
     <row r="207" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B207" s="18">
         <v>44131</v>
@@ -7213,7 +7303,7 @@
     </row>
     <row r="208" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B208" s="18">
         <v>44131</v>
@@ -7259,7 +7349,7 @@
     </row>
     <row r="209" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B209" s="18">
         <v>44131</v>
@@ -7273,7 +7363,7 @@
     </row>
     <row r="210" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B210" s="18">
         <v>44131</v>
@@ -7287,7 +7377,7 @@
     </row>
     <row r="211" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A211" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B211" s="18">
         <v>44138</v>
@@ -7299,7 +7389,7 @@
         <v>5.7511243200634601</v>
       </c>
       <c r="F211" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G211" s="15">
         <f>AVERAGE(D211:D212)</f>
@@ -7336,7 +7426,7 @@
     </row>
     <row r="212" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B212" s="18">
         <v>44138</v>
@@ -7348,12 +7438,12 @@
         <v>5.9365587970394902</v>
       </c>
       <c r="F212" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="213" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B213" s="18">
         <v>44138</v>
@@ -7365,7 +7455,7 @@
         <v>5.8095869664731401</v>
       </c>
       <c r="F213" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G213" s="15">
         <f>AVERAGE(D213:D214)</f>
@@ -7402,7 +7492,7 @@
     </row>
     <row r="214" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B214" s="18">
         <v>44138</v>
@@ -7414,12 +7504,12 @@
         <v>5.6138999922220298</v>
       </c>
       <c r="F214" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="215" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A215" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B215" s="18">
         <v>44138</v>
@@ -7431,7 +7521,7 @@
         <v>5.7977627439042001</v>
       </c>
       <c r="F215" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G215" s="15">
         <f>AVERAGE(D215:D216)</f>
@@ -7468,7 +7558,7 @@
     </row>
     <row r="216" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A216" s="14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B216" s="18">
         <v>44138</v>
@@ -7480,12 +7570,12 @@
         <v>5.8344527805157096</v>
       </c>
       <c r="F216" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="217" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B217" s="18">
         <v>44138</v>
@@ -7497,7 +7587,7 @@
         <v>5.8359057516639998</v>
       </c>
       <c r="F217" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G217" s="15">
         <f>AVERAGE(D217:D218)</f>
@@ -7534,7 +7624,7 @@
     </row>
     <row r="218" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B218" s="18">
         <v>44138</v>
@@ -7546,12 +7636,12 @@
         <v>5.8067328031253398</v>
       </c>
       <c r="F218" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="219" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" s="14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B219" s="18">
         <v>44138</v>
@@ -7563,12 +7653,12 @@
         <v>5.7828991259926301</v>
       </c>
       <c r="F219" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="220" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A220" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B220" s="18">
         <v>44138</v>
@@ -7580,7 +7670,7 @@
         <v>5.7875348110248703</v>
       </c>
       <c r="F220" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G220" s="15">
         <f>AVERAGE(D220:D221)</f>
@@ -7617,7 +7707,7 @@
     </row>
     <row r="221" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B221" s="18">
         <v>44138</v>
@@ -7629,12 +7719,12 @@
         <v>5.8593923969062498</v>
       </c>
       <c r="F221" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="222" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A222" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B222" s="18">
         <v>44138</v>
@@ -7646,7 +7736,7 @@
         <v>5.8637971331942902</v>
       </c>
       <c r="F222" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G222" s="15">
         <f>AVERAGE(D222:D223)</f>
@@ -7683,7 +7773,7 @@
     </row>
     <row r="223" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A223" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B223" s="18">
         <v>44138</v>
@@ -7695,12 +7785,12 @@
         <v>5.9216447305250997</v>
       </c>
       <c r="F223" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="224" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A224" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B224" s="18">
         <v>44138</v>
@@ -7712,7 +7802,7 @@
         <v>5.8308935413871303</v>
       </c>
       <c r="F224" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G224" s="15">
         <f>AVERAGE(D224:D225)</f>
@@ -7749,7 +7839,7 @@
     </row>
     <row r="225" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A225" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B225" s="18">
         <v>44138</v>
@@ -7761,12 +7851,12 @@
         <v>5.6147146386722699</v>
       </c>
       <c r="F225" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="226" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A226" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B226" s="18">
         <v>44138</v>
@@ -7778,7 +7868,7 @@
         <v>5.8198791673243004</v>
       </c>
       <c r="F226" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G226" s="15">
         <f>AVERAGE(D226:D227)</f>
@@ -7815,7 +7905,7 @@
     </row>
     <row r="227" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B227" s="18">
         <v>44138</v>
@@ -7827,12 +7917,12 @@
         <v>5.78140131775206</v>
       </c>
       <c r="F227" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="228" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B228" s="18">
         <v>44138</v>
@@ -7844,12 +7934,12 @@
         <v>5.8401541898225098</v>
       </c>
       <c r="F228" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="229" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B229" s="18">
         <v>44144</v>
@@ -7895,7 +7985,7 @@
     </row>
     <row r="230" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B230" s="18">
         <v>44144</v>
@@ -7909,7 +7999,7 @@
     </row>
     <row r="231" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B231" s="18">
         <v>44144</v>
@@ -7955,7 +8045,7 @@
     </row>
     <row r="232" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B232" s="18">
         <v>44144</v>
@@ -7969,7 +8059,7 @@
     </row>
     <row r="233" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B233" s="18">
         <v>44144</v>
@@ -8015,7 +8105,7 @@
     </row>
     <row r="234" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B234" s="18">
         <v>44144</v>
@@ -8029,7 +8119,7 @@
     </row>
     <row r="235" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B235" s="18">
         <v>44144</v>
@@ -8075,7 +8165,7 @@
     </row>
     <row r="236" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B236" s="18">
         <v>44144</v>
@@ -8089,7 +8179,7 @@
     </row>
     <row r="237" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B237" s="18">
         <v>44144</v>
@@ -8135,7 +8225,7 @@
     </row>
     <row r="238" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B238" s="18">
         <v>44144</v>
@@ -8149,7 +8239,7 @@
     </row>
     <row r="239" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="14" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B239" s="18">
         <v>44144</v>
@@ -8195,7 +8285,7 @@
     </row>
     <row r="240" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B240" s="18">
         <v>44144</v>
@@ -8209,7 +8299,7 @@
     </row>
     <row r="241" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B241" s="18">
         <v>44145</v>
@@ -8223,7 +8313,7 @@
     </row>
     <row r="242" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B242" s="18">
         <v>44145</v>
@@ -8255,21 +8345,21 @@
         <v>1.4336722280464597E-4</v>
       </c>
       <c r="L242" s="15">
-        <f>MIN(D242:D243)</f>
+        <f>MIN(D242:D248)</f>
         <v>7.8751451622983097</v>
       </c>
       <c r="M242" s="15">
-        <f>MAX(D242:D243)</f>
-        <v>7.87820718412478</v>
+        <f>MAX(D242:D248)</f>
+        <v>7.8782839673411598</v>
       </c>
       <c r="N242" s="14">
         <f>M242-L242</f>
-        <v>3.062021826470307E-3</v>
+        <v>3.1388050428500236E-3</v>
       </c>
     </row>
     <row r="243" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B243" s="18">
         <v>44145</v>
@@ -8283,7 +8373,7 @@
     </row>
     <row r="244" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B244" s="18">
         <v>44145</v>
@@ -8297,7 +8387,7 @@
     </row>
     <row r="245" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B245" s="18">
         <v>44145</v>
@@ -8311,7 +8401,7 @@
     </row>
     <row r="246" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B246" s="18">
         <v>44145</v>
@@ -8325,7 +8415,7 @@
     </row>
     <row r="247" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B247" s="18">
         <v>44145</v>
@@ -8339,7 +8429,7 @@
     </row>
     <row r="248" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B248" s="18">
         <v>44145</v>
@@ -8353,7 +8443,7 @@
     </row>
     <row r="249" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B249" s="18">
         <v>44152</v>
@@ -8369,37 +8459,37 @@
         <v>7.9643186141655136</v>
       </c>
       <c r="H249" s="14">
-        <f>_xlfn.STDEV.S(D249:D250)</f>
-        <v>3.3772581975410188E-4</v>
+        <f>_xlfn.STDEV.S(D249:D251)</f>
+        <v>1.5369718495734379E-3</v>
       </c>
       <c r="I249" s="14">
         <f>2*H249</f>
-        <v>6.7545163950820375E-4</v>
+        <v>3.0739436991468758E-3</v>
       </c>
       <c r="J249" s="14">
         <f>H249/G249</f>
-        <v>4.2404860492825495E-5</v>
+        <v>1.9298221530712566E-4</v>
       </c>
       <c r="K249" s="19">
         <f>J249</f>
-        <v>4.2404860492825495E-5</v>
+        <v>1.9298221530712566E-4</v>
       </c>
       <c r="L249" s="15">
-        <f>MIN(D249:D250)</f>
-        <v>7.9649564003244899</v>
+        <f>MIN(D249:D251)</f>
+        <v>7.9625654254129001</v>
       </c>
       <c r="M249" s="15">
-        <f>MAX(D249:D250)</f>
+        <f>MAX(D249:D251)</f>
         <v>7.9654340167591497</v>
       </c>
       <c r="N249" s="14">
         <f>M249-L249</f>
-        <v>4.7761643465982218E-4</v>
+        <v>2.868591346249616E-3</v>
       </c>
     </row>
     <row r="250" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B250" s="18">
         <v>44152</v>
@@ -8413,7 +8503,7 @@
     </row>
     <row r="251" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B251" s="18">
         <v>44152</v>
@@ -8427,7 +8517,7 @@
     </row>
     <row r="252" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B252" s="18">
         <v>44152</v>
@@ -8443,37 +8533,37 @@
         <v>7.9492016477328109</v>
       </c>
       <c r="H252" s="14">
-        <f>_xlfn.STDEV.S(D252:D253)</f>
-        <v>1.3703611034800694E-3</v>
+        <f>_xlfn.STDEV.S(D252:D254)</f>
+        <v>1.2154186460813729E-3</v>
       </c>
       <c r="I252" s="14">
         <f>2*H252</f>
-        <v>2.7407222069601388E-3</v>
+        <v>2.4308372921627457E-3</v>
       </c>
       <c r="J252" s="14">
         <f>H252/G252</f>
-        <v>1.7238977751569677E-4</v>
+        <v>1.5289820285638647E-4</v>
       </c>
       <c r="K252" s="19">
         <f>J252</f>
-        <v>1.7238977751569677E-4</v>
+        <v>1.5289820285638647E-4</v>
       </c>
       <c r="L252" s="15">
-        <f>MIN(D252:D253)</f>
-        <v>7.9486562509213803</v>
+        <f>MIN(D252:D254)</f>
+        <v>7.9483544580977803</v>
       </c>
       <c r="M252" s="15">
-        <f>MAX(D252:D253)</f>
+        <f>MAX(D252:D254)</f>
         <v>7.9505942341792704</v>
       </c>
       <c r="N252" s="14">
         <f>M252-L252</f>
-        <v>1.9379832578900746E-3</v>
+        <v>2.2397760814900636E-3</v>
       </c>
     </row>
     <row r="253" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B253" s="18">
         <v>44152</v>
@@ -8487,7 +8577,7 @@
     </row>
     <row r="254" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B254" s="18">
         <v>44152</v>
@@ -8501,7 +8591,7 @@
     </row>
     <row r="255" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B255" s="18">
         <v>44152</v>
@@ -8517,37 +8607,37 @@
         <v>7.9256810439087433</v>
       </c>
       <c r="H255" s="14">
-        <f>_xlfn.STDEV.S(D255:D256)</f>
-        <v>1.0994516294491037E-3</v>
+        <f>_xlfn.STDEV.S(D255:D257)</f>
+        <v>2.3538610479866633E-3</v>
       </c>
       <c r="I255" s="14">
         <f>2*H255</f>
-        <v>2.1989032588982074E-3</v>
+        <v>4.7077220959733266E-3</v>
       </c>
       <c r="J255" s="14">
         <f>H255/G255</f>
-        <v>1.3872014573360655E-4</v>
+        <v>2.9699164462285746E-4</v>
       </c>
       <c r="K255" s="19">
         <f>J255</f>
-        <v>1.3872014573360655E-4</v>
+        <v>2.9699164462285746E-4</v>
       </c>
       <c r="L255" s="15">
-        <f>MIN(D255:D256)</f>
-        <v>7.9261863540978297</v>
+        <f>MIN(D255:D257)</f>
+        <v>7.9231155641250304</v>
       </c>
       <c r="M255" s="15">
-        <f>MAX(D255:D256)</f>
+        <f>MAX(D255:D257)</f>
         <v>7.9277412135033698</v>
       </c>
       <c r="N255" s="14">
         <f>M255-L255</f>
-        <v>1.554859405540121E-3</v>
+        <v>4.6256493783394248E-3</v>
       </c>
     </row>
     <row r="256" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B256" s="18">
         <v>44152</v>
@@ -8559,9 +8649,9 @@
         <v>7.7863432043211098</v>
       </c>
     </row>
-    <row r="257" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B257" s="18">
         <v>44152</v>
@@ -8571,6 +8661,336 @@
       </c>
       <c r="E257" s="15">
         <v>7.7832724143483096</v>
+      </c>
+    </row>
+    <row r="258" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="B258" s="18">
+        <v>44293</v>
+      </c>
+      <c r="D258" s="15">
+        <v>7.91769106736231</v>
+      </c>
+      <c r="E258" s="15">
+        <v>7.7259869711707596</v>
+      </c>
+    </row>
+    <row r="259" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="B259" s="18">
+        <v>44293</v>
+      </c>
+      <c r="D259" s="15">
+        <v>7.8873780044373101</v>
+      </c>
+      <c r="E259" s="15">
+        <v>7.69689986478196</v>
+      </c>
+      <c r="G259" s="15">
+        <f>AVERAGE(D259:D262)</f>
+        <v>7.8900805027259455</v>
+      </c>
+      <c r="H259" s="14">
+        <f>_xlfn.STDEV.S(D259:D262)</f>
+        <v>4.3293822891628747E-3</v>
+      </c>
+      <c r="I259" s="14">
+        <f>2*H259</f>
+        <v>8.6587645783257495E-3</v>
+      </c>
+      <c r="J259" s="14">
+        <f>H259/G259</f>
+        <v>5.4871205530375965E-4</v>
+      </c>
+      <c r="K259" s="19">
+        <f>J259</f>
+        <v>5.4871205530375965E-4</v>
+      </c>
+      <c r="L259" s="15">
+        <f>MIN(D259:D262)</f>
+        <v>7.8854160141673102</v>
+      </c>
+      <c r="M259" s="15">
+        <f>MAX(D259:D262)</f>
+        <v>7.8938933307921104</v>
+      </c>
+      <c r="N259" s="14">
+        <f>M259-L259</f>
+        <v>8.4773166248002241E-3</v>
+      </c>
+    </row>
+    <row r="260" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="B260" s="18">
+        <v>44293</v>
+      </c>
+      <c r="D260" s="15">
+        <v>7.8936346615070496</v>
+      </c>
+      <c r="E260" s="15">
+        <v>7.7031565218517004</v>
+      </c>
+    </row>
+    <row r="261" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A261" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="B261" s="18">
+        <v>44293</v>
+      </c>
+      <c r="D261" s="15">
+        <v>7.8854160141673102</v>
+      </c>
+      <c r="E261" s="15">
+        <v>7.6949378745119601</v>
+      </c>
+    </row>
+    <row r="262" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="B262" s="18">
+        <v>44293</v>
+      </c>
+      <c r="D262" s="15">
+        <v>7.8938933307921104</v>
+      </c>
+      <c r="E262" s="15">
+        <v>7.7034151911367603</v>
+      </c>
+    </row>
+    <row r="263" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A263" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="B263" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D263" s="15">
+        <v>8.0949290355521804</v>
+      </c>
+      <c r="E263" s="15">
+        <v>8.0949290355521804</v>
+      </c>
+      <c r="G263" s="15">
+        <f>AVERAGE(D263:D265)</f>
+        <v>8.0927970086849808</v>
+      </c>
+      <c r="H263" s="14">
+        <f>_xlfn.STDEV.S(D263:D265)</f>
+        <v>1.8740549084276918E-3</v>
+      </c>
+      <c r="I263" s="14">
+        <f>2*H263</f>
+        <v>3.7481098168553836E-3</v>
+      </c>
+      <c r="J263" s="14">
+        <f>H263/G263</f>
+        <v>2.315707296768354E-4</v>
+      </c>
+      <c r="K263" s="19">
+        <f>J263</f>
+        <v>2.315707296768354E-4</v>
+      </c>
+      <c r="L263" s="15">
+        <f>MIN(D263:D265)</f>
+        <v>8.0914101715023303</v>
+      </c>
+      <c r="M263" s="15">
+        <f>MAX(D263:D265)</f>
+        <v>8.0949290355521804</v>
+      </c>
+      <c r="N263" s="14">
+        <f>M263-L263</f>
+        <v>3.5188640498500234E-3</v>
+      </c>
+    </row>
+    <row r="264" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A264" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="B264" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D264" s="15">
+        <v>8.0920518190004298</v>
+      </c>
+      <c r="E264" s="15">
+        <v>8.0920518190004298</v>
+      </c>
+    </row>
+    <row r="265" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="B265" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D265" s="15">
+        <v>8.0914101715023303</v>
+      </c>
+      <c r="E265" s="15">
+        <v>8.0914101715023303</v>
+      </c>
+    </row>
+    <row r="266" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="B266" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D266" s="15">
+        <v>7.9785190741932297</v>
+      </c>
+      <c r="E266" s="15">
+        <v>7.7757503268440598</v>
+      </c>
+      <c r="G266" s="15">
+        <f>AVERAGE(D266:D268)</f>
+        <v>7.9736270291428371</v>
+      </c>
+      <c r="H266" s="14">
+        <f>_xlfn.STDEV.S(D266:D268)</f>
+        <v>4.2432062167148277E-3</v>
+      </c>
+      <c r="I266" s="14">
+        <f>2*H266</f>
+        <v>8.4864124334296555E-3</v>
+      </c>
+      <c r="J266" s="14">
+        <f>H266/G266</f>
+        <v>5.3215509092741846E-4</v>
+      </c>
+      <c r="K266" s="19">
+        <f>J266</f>
+        <v>5.3215509092741846E-4</v>
+      </c>
+      <c r="L266" s="15">
+        <f>MIN(D266:D268)</f>
+        <v>7.9709449548939402</v>
+      </c>
+      <c r="M266" s="15">
+        <f>MAX(D266:D268)</f>
+        <v>7.9785190741932297</v>
+      </c>
+      <c r="N266" s="14">
+        <f>M266-L266</f>
+        <v>7.5741192992895279E-3</v>
+      </c>
+    </row>
+    <row r="267" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="B267" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D267" s="15">
+        <v>7.9709449548939402</v>
+      </c>
+      <c r="E267" s="15">
+        <v>7.7681762075447596</v>
+      </c>
+      <c r="F267" s="16" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="268" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A268" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="B268" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D268" s="15">
+        <v>7.9714170583413404</v>
+      </c>
+      <c r="E268" s="15">
+        <v>7.7686483109921696</v>
+      </c>
+      <c r="F268" s="16" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="269" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A269" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="B269" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D269" s="15">
+        <v>7.9951733551669699</v>
+      </c>
+      <c r="E269" s="15">
+        <v>7.8367833080420297</v>
+      </c>
+      <c r="G269" s="15">
+        <f>AVERAGE(D269:D271)</f>
+        <v>7.9959326977794474</v>
+      </c>
+      <c r="H269" s="14">
+        <f>_xlfn.STDEV.S(D269:D271)</f>
+        <v>7.5360260786461783E-4</v>
+      </c>
+      <c r="I269" s="14">
+        <f>2*H269</f>
+        <v>1.5072052157292357E-3</v>
+      </c>
+      <c r="J269" s="14">
+        <f>H269/G269</f>
+        <v>9.4248242994078848E-5</v>
+      </c>
+      <c r="K269" s="19">
+        <f>J269</f>
+        <v>9.4248242994078848E-5</v>
+      </c>
+      <c r="L269" s="15">
+        <f>MIN(D269:D271)</f>
+        <v>7.9951733551669699</v>
+      </c>
+      <c r="M269" s="15">
+        <f>MAX(D269:D271)</f>
+        <v>7.9966804261305002</v>
+      </c>
+      <c r="N269" s="14">
+        <f>M269-L269</f>
+        <v>1.5070709635303103E-3</v>
+      </c>
+    </row>
+    <row r="270" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A270" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="B270" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D270" s="15">
+        <v>7.9966804261305002</v>
+      </c>
+      <c r="E270" s="15">
+        <v>7.8382903790055503</v>
+      </c>
+    </row>
+    <row r="271" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A271" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="B271" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D271" s="15">
+        <v>7.9959443120408702</v>
+      </c>
+      <c r="E271" s="15">
+        <v>7.8375542649159202</v>
       </c>
     </row>
   </sheetData>
@@ -8589,7 +9009,7 @@
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8689,7 +9109,7 @@
         <v>8.1049089149999993</v>
       </c>
       <c r="C3" s="12">
-        <f t="shared" ref="C3:C11" si="0">$L$2</f>
+        <f t="shared" ref="C3:C12" si="0">$L$2</f>
         <v>8.0935490943465993</v>
       </c>
       <c r="D3" s="12">
@@ -8702,7 +9122,7 @@
       </c>
       <c r="G3">
         <f>SQRT(SUM(E2:E46)/ROWS(E2:E46))</f>
-        <v>1.0605002710086344E-2</v>
+        <v>1.0605595320379663E-2</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -8759,7 +9179,7 @@
       </c>
       <c r="G5">
         <f>SQRT(G3^2+G4^2)</f>
-        <v>1.1021165205228471E-2</v>
+        <v>1.1021735439560278E-2</v>
       </c>
       <c r="H5" t="s">
         <v>32</v>
@@ -8768,7 +9188,7 @@
         <v>28</v>
       </c>
       <c r="K5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -8792,7 +9212,7 @@
       </c>
       <c r="G6">
         <f>G5/L2</f>
-        <v>1.3617221662282659E-3</v>
+        <v>1.3617926216397498E-3</v>
       </c>
       <c r="H6" t="s">
         <v>31</v>
@@ -8883,9 +9303,9 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>297</v>
-      </c>
-      <c r="B11" s="25">
+        <v>296</v>
+      </c>
+      <c r="B11" s="27">
         <v>8.1335197047369494</v>
       </c>
       <c r="C11" s="12">
@@ -8902,9 +9322,24 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="26"/>
+      <c r="A12" s="24" t="s">
+        <v>330</v>
+      </c>
+      <c r="B12" s="27">
+        <v>8.0927970086849808</v>
+      </c>
+      <c r="C12" s="12">
+        <f t="shared" si="0"/>
+        <v>8.0935490943465993</v>
+      </c>
+      <c r="D12" s="12">
+        <f t="shared" ref="D12" si="3">B12-C12</f>
+        <v>-7.5208566161855117E-4</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" ref="E12" si="4">D12^2</f>
+        <v>5.6563284241221383E-7</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
@@ -9113,7 +9548,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9124,14 +9559,14 @@
     <col min="4" max="4" width="12.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="70.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="103" style="6" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="9" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" style="10" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -9139,7 +9574,7 @@
         <v>40</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C1" t="s">
         <v>34</v>
@@ -9151,6 +9586,9 @@
         <v>35</v>
       </c>
       <c r="F1" s="5"/>
+      <c r="G1" t="s">
+        <v>331</v>
+      </c>
       <c r="J1" s="8"/>
       <c r="K1" t="s">
         <v>241</v>
@@ -9186,15 +9624,15 @@
       </c>
       <c r="F2" s="5"/>
       <c r="G2">
-        <f>SQRT(SUM(E2:E12)/ROWS(E2:E12))</f>
-        <v>8.2271234099468363E-2</v>
+        <f>SQRT(SUM(E2:E14)/ROWS(E2:E14))</f>
+        <v>8.1497754965428576E-2</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" t="s">
-        <v>242</v>
+        <v>332</v>
       </c>
       <c r="L2" s="10">
         <v>7.8738051640000002</v>
@@ -9214,7 +9652,7 @@
         <v>7.872094111</v>
       </c>
       <c r="C3" s="12">
-        <f t="shared" ref="C3:C12" si="2">$L$2</f>
+        <f t="shared" ref="C3:C14" si="2">$L$2</f>
         <v>7.8738051640000002</v>
       </c>
       <c r="D3" s="12">
@@ -9232,7 +9670,19 @@
         <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>244</v>
+        <v>243</v>
+      </c>
+      <c r="K3" t="s">
+        <v>333</v>
+      </c>
+      <c r="L3" s="10">
+        <v>7.9959326977794474</v>
+      </c>
+      <c r="M3" s="10">
+        <v>30.34</v>
+      </c>
+      <c r="N3" s="10">
+        <v>14.11</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -9256,7 +9706,7 @@
       </c>
       <c r="G4">
         <f>SQRT(G2^2+G3^2)</f>
-        <v>8.2325913054454039E-2</v>
+        <v>8.1552952518011507E-2</v>
       </c>
       <c r="H4" t="s">
         <v>32</v>
@@ -9286,7 +9736,7 @@
       </c>
       <c r="G5">
         <f>G4/L2</f>
-        <v>1.0455670586168194E-2</v>
+        <v>1.0357501972601707E-2</v>
       </c>
       <c r="H5" t="s">
         <v>31</v>
@@ -9436,14 +9886,44 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
+      <c r="A13" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="B13" s="12">
+        <v>7.91769106736231</v>
+      </c>
+      <c r="C13" s="12">
+        <f t="shared" si="2"/>
+        <v>7.8738051640000002</v>
+      </c>
+      <c r="D13" s="12">
+        <f t="shared" ref="D13:D14" si="3">B13-C13</f>
+        <v>4.3885903362309797E-2</v>
+      </c>
+      <c r="E13" s="13">
+        <f t="shared" ref="E13:E14" si="4">D13^2</f>
+        <v>1.9259725139259944E-3</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
+      <c r="A14" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="B14" s="12">
+        <v>7.9736270291428371</v>
+      </c>
+      <c r="C14" s="12">
+        <f t="shared" si="2"/>
+        <v>7.8738051640000002</v>
+      </c>
+      <c r="D14" s="12">
+        <f t="shared" si="3"/>
+        <v>9.9821865142836863E-2</v>
+      </c>
+      <c r="E14" s="13">
+        <f t="shared" si="4"/>
+        <v>9.9644047605947084E-3</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>

</xml_diff>

<commit_message>
Compiled Christian's pH data. All look good with a coefficient of variation less than 1 % (0.26% max)
</commit_message>
<xml_diff>
--- a/check sample work/pH QAQC/20210326 pH check sample results summary.xlsx
+++ b/check sample work/pH QAQC/20210326 pH check sample results summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rye-Tech\Documents\R\rye-tech-home\2021-season-summary\check sample work\pH QAQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6152E834-7FA6-4BBA-ABCF-981BC9497B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96CA47B-E28A-49A9-802E-EFB50DF5BD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="379">
   <si>
     <t>sample</t>
   </si>
@@ -1033,6 +1033,141 @@
   </si>
   <si>
     <t>Batch 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BAYSTD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H2-702-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H2-702-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H2-702-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H3-702-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H3-702-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H3-702-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H2-719-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H2-719-2</t>
+  </si>
+  <si>
+    <t>Christian's Samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BaySTD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H3-719-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H3-719-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T44-702-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T44-702-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T4-702-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T4-702-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T3-702-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T3-702-2</t>
+  </si>
+  <si>
+    <t>Bay Standard Batch 2 ran from here on out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mislabeled CRM 186, when it is TRIS Buffer </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T6-702-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T6-702-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T27-719-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T27-719-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T10-719-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T10-719-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T36-719-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T36-719-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T16-719-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T16-719-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T12-708-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T12-708-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T6-708-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T6-708-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T20-708-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T20-708-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T8-714-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T8-714-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T14-714-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T14-714-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T38-714-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T38-714-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T21-708-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T21-708-2</t>
   </si>
 </sst>
 </file>
@@ -2245,11 +2380,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O271"/>
+  <dimension ref="A1:O316"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A263" sqref="A263"/>
+      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O304" sqref="O304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8767,230 +8902,1594 @@
     </row>
     <row r="263" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="14" t="s">
-        <v>319</v>
+        <v>334</v>
       </c>
       <c r="B263" s="18">
-        <v>44313</v>
+        <v>44306</v>
       </c>
       <c r="D263" s="15">
-        <v>8.0949290355521804</v>
+        <v>7.9494492721433501</v>
       </c>
       <c r="E263" s="15">
-        <v>8.0949290355521804</v>
-      </c>
-      <c r="G263" s="15">
-        <f>AVERAGE(D263:D265)</f>
-        <v>8.0927970086849808</v>
-      </c>
-      <c r="H263" s="14">
-        <f>_xlfn.STDEV.S(D263:D265)</f>
-        <v>1.8740549084276918E-3</v>
-      </c>
-      <c r="I263" s="14">
-        <f>2*H263</f>
-        <v>3.7481098168553836E-3</v>
-      </c>
-      <c r="J263" s="14">
-        <f>H263/G263</f>
-        <v>2.315707296768354E-4</v>
-      </c>
-      <c r="K263" s="19">
-        <f>J263</f>
-        <v>2.315707296768354E-4</v>
-      </c>
-      <c r="L263" s="15">
-        <f>MIN(D263:D265)</f>
-        <v>8.0914101715023303</v>
-      </c>
-      <c r="M263" s="15">
-        <f>MAX(D263:D265)</f>
-        <v>8.0949290355521804</v>
-      </c>
-      <c r="N263" s="14">
-        <f>M263-L263</f>
-        <v>3.5188640498500234E-3</v>
+        <v>7.7577451759517997</v>
       </c>
     </row>
     <row r="264" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="14" t="s">
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="B264" s="18">
-        <v>44313</v>
+        <v>44306</v>
       </c>
       <c r="D264" s="15">
-        <v>8.0920518190004298</v>
+        <v>7.5152311248429502</v>
       </c>
       <c r="E264" s="15">
-        <v>8.0920518190004298</v>
+        <v>7.41933030462563</v>
+      </c>
+      <c r="F264" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G264" s="15">
+        <f>AVERAGE(D264:D266)</f>
+        <v>7.4845624190066138</v>
+      </c>
+      <c r="H264" s="14">
+        <f>_xlfn.STDEV.S(D264:D266)</f>
+        <v>4.8362899545540926E-2</v>
+      </c>
+      <c r="I264" s="14">
+        <f>2*H264</f>
+        <v>9.6725799091081852E-2</v>
+      </c>
+      <c r="J264" s="14">
+        <f>H264/G264</f>
+        <v>6.4616869815563478E-3</v>
+      </c>
+      <c r="K264" s="19">
+        <f>J264</f>
+        <v>6.4616869815563478E-3</v>
+      </c>
+      <c r="L264" s="15">
+        <f>MIN(D264:D266)</f>
+        <v>7.42881095443762</v>
+      </c>
+      <c r="M264" s="15">
+        <f>MAX(D264:D266)</f>
+        <v>7.5152311248429502</v>
+      </c>
+      <c r="N264" s="14">
+        <f>M264-L264</f>
+        <v>8.6420170405330232E-2</v>
       </c>
     </row>
     <row r="265" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="14" t="s">
-        <v>321</v>
+        <v>336</v>
       </c>
       <c r="B265" s="18">
-        <v>44313</v>
+        <v>44306</v>
       </c>
       <c r="D265" s="15">
-        <v>8.0914101715023303</v>
+        <v>7.5096451777392703</v>
       </c>
       <c r="E265" s="15">
-        <v>8.0914101715023303</v>
+        <v>7.4137443575219502</v>
+      </c>
+      <c r="F265" s="16" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="266" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="14" t="s">
-        <v>322</v>
+        <v>337</v>
       </c>
       <c r="B266" s="18">
-        <v>44313</v>
+        <v>44306</v>
       </c>
       <c r="D266" s="15">
-        <v>7.9785190741932297</v>
+        <v>7.42881095443762</v>
       </c>
       <c r="E266" s="15">
-        <v>7.7757503268440598</v>
-      </c>
-      <c r="G266" s="15">
-        <f>AVERAGE(D266:D268)</f>
-        <v>7.9736270291428371</v>
-      </c>
-      <c r="H266" s="14">
-        <f>_xlfn.STDEV.S(D266:D268)</f>
-        <v>4.2432062167148277E-3</v>
-      </c>
-      <c r="I266" s="14">
-        <f>2*H266</f>
-        <v>8.4864124334296555E-3</v>
-      </c>
-      <c r="J266" s="14">
-        <f>H266/G266</f>
-        <v>5.3215509092741846E-4</v>
-      </c>
-      <c r="K266" s="19">
-        <f>J266</f>
-        <v>5.3215509092741846E-4</v>
-      </c>
-      <c r="L266" s="15">
-        <f>MIN(D266:D268)</f>
-        <v>7.9709449548939402</v>
-      </c>
-      <c r="M266" s="15">
-        <f>MAX(D266:D268)</f>
-        <v>7.9785190741932297</v>
-      </c>
-      <c r="N266" s="14">
-        <f>M266-L266</f>
-        <v>7.5741192992895279E-3</v>
+        <v>7.3329101342202998</v>
+      </c>
+      <c r="F266" s="16" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="267" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="14" t="s">
-        <v>323</v>
+        <v>338</v>
       </c>
       <c r="B267" s="18">
-        <v>44313</v>
+        <v>44306</v>
       </c>
       <c r="D267" s="15">
-        <v>7.9709449548939402</v>
+        <v>7.7909449508084103</v>
       </c>
       <c r="E267" s="15">
-        <v>7.7681762075447596</v>
+        <v>7.6822482668969503</v>
       </c>
       <c r="F267" s="16" t="s">
-        <v>328</v>
+        <v>343</v>
+      </c>
+      <c r="G267" s="15">
+        <f>AVERAGE(D267:D269)</f>
+        <v>7.7919848702495003</v>
+      </c>
+      <c r="H267" s="14">
+        <f>_xlfn.STDEV.S(D267:D269)</f>
+        <v>9.0144820968213494E-4</v>
+      </c>
+      <c r="I267" s="14">
+        <f>2*H267</f>
+        <v>1.8028964193642699E-3</v>
+      </c>
+      <c r="J267" s="14">
+        <f>H267/G267</f>
+        <v>1.1568916324824313E-4</v>
+      </c>
+      <c r="K267" s="19">
+        <f>J267</f>
+        <v>1.1568916324824313E-4</v>
+      </c>
+      <c r="L267" s="15">
+        <f>MIN(D267:D269)</f>
+        <v>7.7909449508084103</v>
+      </c>
+      <c r="M267" s="15">
+        <f>MAX(D267:D269)</f>
+        <v>7.7925440031977899</v>
+      </c>
+      <c r="N267" s="14">
+        <f>M267-L267</f>
+        <v>1.5990523893796293E-3</v>
       </c>
     </row>
     <row r="268" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="14" t="s">
-        <v>324</v>
+        <v>339</v>
       </c>
       <c r="B268" s="18">
-        <v>44313</v>
+        <v>44306</v>
       </c>
       <c r="D268" s="15">
-        <v>7.9714170583413404</v>
+        <v>7.7925440031977899</v>
       </c>
       <c r="E268" s="15">
-        <v>7.7686483109921696</v>
+        <v>7.6845847885638596</v>
       </c>
       <c r="F268" s="16" t="s">
-        <v>328</v>
+        <v>343</v>
       </c>
     </row>
     <row r="269" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="14" t="s">
-        <v>325</v>
+        <v>340</v>
       </c>
       <c r="B269" s="18">
-        <v>44313</v>
+        <v>44306</v>
       </c>
       <c r="D269" s="15">
-        <v>7.9951733551669699</v>
+        <v>7.7924656567422996</v>
       </c>
       <c r="E269" s="15">
-        <v>7.8367833080420297</v>
-      </c>
-      <c r="G269" s="15">
-        <f>AVERAGE(D269:D271)</f>
-        <v>7.9959326977794474</v>
-      </c>
-      <c r="H269" s="14">
-        <f>_xlfn.STDEV.S(D269:D271)</f>
-        <v>7.5360260786461783E-4</v>
-      </c>
-      <c r="I269" s="14">
-        <f>2*H269</f>
-        <v>1.5072052157292357E-3</v>
-      </c>
-      <c r="J269" s="14">
-        <f>H269/G269</f>
-        <v>9.4248242994078848E-5</v>
-      </c>
-      <c r="K269" s="19">
-        <f>J269</f>
-        <v>9.4248242994078848E-5</v>
-      </c>
-      <c r="L269" s="15">
-        <f>MIN(D269:D271)</f>
-        <v>7.9951733551669699</v>
-      </c>
-      <c r="M269" s="15">
-        <f>MAX(D269:D271)</f>
-        <v>7.9966804261305002</v>
-      </c>
-      <c r="N269" s="14">
-        <f>M269-L269</f>
-        <v>1.5070709635303103E-3</v>
+        <v>7.6846539055161598</v>
+      </c>
+      <c r="F269" s="16" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="270" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="14" t="s">
-        <v>326</v>
+        <v>341</v>
       </c>
       <c r="B270" s="18">
-        <v>44313</v>
+        <v>44306</v>
       </c>
       <c r="D270" s="15">
-        <v>7.9966804261305002</v>
+        <v>7.7692146741796799</v>
       </c>
       <c r="E270" s="15">
-        <v>7.8382903790055503</v>
+        <v>7.6382752903317197</v>
+      </c>
+      <c r="F270" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G270" s="15">
+        <f>AVERAGE(D270:D271)</f>
+        <v>7.7517480588763394</v>
+      </c>
+      <c r="H270" s="14">
+        <f>_xlfn.STDEV.S(D270:D271)</f>
+        <v>2.4701524250736934E-2</v>
+      </c>
+      <c r="I270" s="14">
+        <f>2*H270</f>
+        <v>4.9403048501473867E-2</v>
+      </c>
+      <c r="J270" s="14">
+        <f>H270/G270</f>
+        <v>3.1865747007156424E-3</v>
+      </c>
+      <c r="K270" s="19">
+        <f>J270</f>
+        <v>3.1865747007156424E-3</v>
+      </c>
+      <c r="L270" s="15">
+        <f>MIN(D270:D271)</f>
+        <v>7.7342814435729998</v>
+      </c>
+      <c r="M270" s="15">
+        <f>MAX(D270:D271)</f>
+        <v>7.7692146741796799</v>
+      </c>
+      <c r="N270" s="14">
+        <f>M270-L270</f>
+        <v>3.4933230606680077E-2</v>
       </c>
     </row>
     <row r="271" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="B271" s="18">
+        <v>44306</v>
+      </c>
+      <c r="D271" s="15">
+        <v>7.7342814435729998</v>
+      </c>
+      <c r="E271" s="15">
+        <v>7.6033420597250396</v>
+      </c>
+      <c r="F271" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="272" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A272" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="B272" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D272" s="15">
+        <v>8.0949290355521804</v>
+      </c>
+      <c r="E272" s="15">
+        <v>8.0949290355521804</v>
+      </c>
+      <c r="F272" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="G272" s="15">
+        <f>AVERAGE(D272:D274)</f>
+        <v>8.0927970086849808</v>
+      </c>
+      <c r="H272" s="14">
+        <f>_xlfn.STDEV.S(D272:D274)</f>
+        <v>1.8740549084276918E-3</v>
+      </c>
+      <c r="I272" s="14">
+        <f>2*H272</f>
+        <v>3.7481098168553836E-3</v>
+      </c>
+      <c r="J272" s="14">
+        <f>H272/G272</f>
+        <v>2.315707296768354E-4</v>
+      </c>
+      <c r="K272" s="19">
+        <f>J272</f>
+        <v>2.315707296768354E-4</v>
+      </c>
+      <c r="L272" s="15">
+        <f>MIN(D272:D274)</f>
+        <v>8.0914101715023303</v>
+      </c>
+      <c r="M272" s="15">
+        <f>MAX(D272:D274)</f>
+        <v>8.0949290355521804</v>
+      </c>
+      <c r="N272" s="14">
+        <f>M272-L272</f>
+        <v>3.5188640498500234E-3</v>
+      </c>
+    </row>
+    <row r="273" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A273" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="B273" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D273" s="15">
+        <v>8.0920518190004298</v>
+      </c>
+      <c r="E273" s="15">
+        <v>8.0920518190004298</v>
+      </c>
+    </row>
+    <row r="274" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A274" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="B274" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D274" s="15">
+        <v>8.0914101715023303</v>
+      </c>
+      <c r="E274" s="15">
+        <v>8.0914101715023303</v>
+      </c>
+    </row>
+    <row r="275" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A275" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="B275" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D275" s="15">
+        <v>7.9785190741932297</v>
+      </c>
+      <c r="E275" s="15">
+        <v>7.7757503268440598</v>
+      </c>
+      <c r="G275" s="15">
+        <f>AVERAGE(D275:D277)</f>
+        <v>7.9736270291428371</v>
+      </c>
+      <c r="H275" s="14">
+        <f>_xlfn.STDEV.S(D275:D277)</f>
+        <v>4.2432062167148277E-3</v>
+      </c>
+      <c r="I275" s="14">
+        <f>2*H275</f>
+        <v>8.4864124334296555E-3</v>
+      </c>
+      <c r="J275" s="14">
+        <f>H275/G275</f>
+        <v>5.3215509092741846E-4</v>
+      </c>
+      <c r="K275" s="19">
+        <f>J275</f>
+        <v>5.3215509092741846E-4</v>
+      </c>
+      <c r="L275" s="15">
+        <f>MIN(D275:D277)</f>
+        <v>7.9709449548939402</v>
+      </c>
+      <c r="M275" s="15">
+        <f>MAX(D275:D277)</f>
+        <v>7.9785190741932297</v>
+      </c>
+      <c r="N275" s="14">
+        <f>M275-L275</f>
+        <v>7.5741192992895279E-3</v>
+      </c>
+    </row>
+    <row r="276" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A276" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="B276" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D276" s="15">
+        <v>7.9709449548939402</v>
+      </c>
+      <c r="E276" s="15">
+        <v>7.7681762075447596</v>
+      </c>
+      <c r="F276" s="16" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="277" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A277" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="B277" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D277" s="15">
+        <v>7.9714170583413404</v>
+      </c>
+      <c r="E277" s="15">
+        <v>7.7686483109921696</v>
+      </c>
+      <c r="F277" s="16" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="278" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A278" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="B278" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D278" s="15">
+        <v>7.9951733551669699</v>
+      </c>
+      <c r="E278" s="15">
+        <v>7.8367833080420297</v>
+      </c>
+      <c r="G278" s="15">
+        <f>AVERAGE(D278:D280)</f>
+        <v>7.9959326977794474</v>
+      </c>
+      <c r="H278" s="14">
+        <f>_xlfn.STDEV.S(D278:D280)</f>
+        <v>7.5360260786461783E-4</v>
+      </c>
+      <c r="I278" s="14">
+        <f>2*H278</f>
+        <v>1.5072052157292357E-3</v>
+      </c>
+      <c r="J278" s="14">
+        <f>H278/G278</f>
+        <v>9.4248242994078848E-5</v>
+      </c>
+      <c r="K278" s="19">
+        <f>J278</f>
+        <v>9.4248242994078848E-5</v>
+      </c>
+      <c r="L278" s="15">
+        <f>MIN(D278:D280)</f>
+        <v>7.9951733551669699</v>
+      </c>
+      <c r="M278" s="15">
+        <f>MAX(D278:D280)</f>
+        <v>7.9966804261305002</v>
+      </c>
+      <c r="N278" s="14">
+        <f>M278-L278</f>
+        <v>1.5070709635303103E-3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A279" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="B279" s="18">
+        <v>44313</v>
+      </c>
+      <c r="D279" s="15">
+        <v>7.9966804261305002</v>
+      </c>
+      <c r="E279" s="15">
+        <v>7.8382903790055503</v>
+      </c>
+    </row>
+    <row r="280" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A280" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="B271" s="18">
+      <c r="B280" s="18">
         <v>44313</v>
       </c>
-      <c r="D271" s="15">
+      <c r="D280" s="15">
         <v>7.9959443120408702</v>
       </c>
-      <c r="E271" s="15">
+      <c r="E280" s="15">
         <v>7.8375542649159202</v>
+      </c>
+    </row>
+    <row r="281" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A281" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="B281" s="18">
+        <v>44314</v>
+      </c>
+      <c r="D281" s="15">
+        <v>7.9990152489302302</v>
+      </c>
+      <c r="E281" s="15">
+        <v>7.84062520180529</v>
+      </c>
+      <c r="F281" s="16" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="282" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A282" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="B282" s="18">
+        <v>44314</v>
+      </c>
+      <c r="D282" s="15">
+        <v>7.8524167257787196</v>
+      </c>
+      <c r="E282" s="15">
+        <v>7.7214773419307603</v>
+      </c>
+      <c r="F282" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G282" s="15">
+        <f>AVERAGE(D282:D283)</f>
+        <v>7.8642746748035552</v>
+      </c>
+      <c r="H282" s="14">
+        <f>_xlfn.STDEV.S(D282:D283)</f>
+        <v>1.6769672332850712E-2</v>
+      </c>
+      <c r="I282" s="14">
+        <f>2*H282</f>
+        <v>3.3539344665701423E-2</v>
+      </c>
+      <c r="J282" s="14">
+        <f>H282/G282</f>
+        <v>2.132386396240618E-3</v>
+      </c>
+      <c r="K282" s="19">
+        <f>J282</f>
+        <v>2.132386396240618E-3</v>
+      </c>
+      <c r="L282" s="15">
+        <f>MIN(D282:D283)</f>
+        <v>7.8524167257787196</v>
+      </c>
+      <c r="M282" s="15">
+        <f>MAX(D282:D283)</f>
+        <v>7.87613262382839</v>
+      </c>
+      <c r="N282" s="14">
+        <f>M282-L282</f>
+        <v>2.3715898049670336E-2</v>
+      </c>
+    </row>
+    <row r="283" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A283" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="B283" s="18">
+        <v>44314</v>
+      </c>
+      <c r="D283" s="15">
+        <v>7.87613262382839</v>
+      </c>
+      <c r="E283" s="15">
+        <v>7.7451932399804297</v>
+      </c>
+      <c r="F283" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="284" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A284" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="B284" s="18">
+        <v>44314</v>
+      </c>
+      <c r="D284" s="15">
+        <v>8.0270017826068294</v>
+      </c>
+      <c r="E284" s="15">
+        <v>7.9163864903357499</v>
+      </c>
+      <c r="F284" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G284" s="15">
+        <f>AVERAGE(D284:D285)</f>
+        <v>8.0343987753136794</v>
+      </c>
+      <c r="H284" s="14">
+        <f>_xlfn.STDEV.S(D284:D285)</f>
+        <v>1.0460927406802161E-2</v>
+      </c>
+      <c r="I284" s="14">
+        <f>2*H284</f>
+        <v>2.0921854813604323E-2</v>
+      </c>
+      <c r="J284" s="14">
+        <f>H284/G284</f>
+        <v>1.3020174501350594E-3</v>
+      </c>
+      <c r="K284" s="19">
+        <f>J284</f>
+        <v>1.3020174501350594E-3</v>
+      </c>
+      <c r="L284" s="15">
+        <f>MIN(D284:D285)</f>
+        <v>8.0270017826068294</v>
+      </c>
+      <c r="M284" s="15">
+        <f>MAX(D284:D285)</f>
+        <v>8.0417957680205294</v>
+      </c>
+      <c r="N284" s="14">
+        <f>M284-L284</f>
+        <v>1.4793985413700028E-2</v>
+      </c>
+    </row>
+    <row r="285" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A285" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="B285" s="18">
+        <v>44314</v>
+      </c>
+      <c r="D285" s="15">
+        <v>8.0417957680205294</v>
+      </c>
+      <c r="E285" s="15">
+        <v>7.93118047574945</v>
+      </c>
+      <c r="F285" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="286" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A286" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="B286" s="18">
+        <v>44314</v>
+      </c>
+      <c r="D286" s="15">
+        <v>8.1516851934779702</v>
+      </c>
+      <c r="E286" s="15">
+        <v>8.0308577011271591</v>
+      </c>
+      <c r="F286" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G286" s="15">
+        <f>AVERAGE(D286:D287)</f>
+        <v>8.1440876812748453</v>
+      </c>
+      <c r="H286" s="14">
+        <f>_xlfn.STDEV.S(D286:D287)</f>
+        <v>1.0744504797954297E-2</v>
+      </c>
+      <c r="I286" s="14">
+        <f>2*H286</f>
+        <v>2.1489009595908593E-2</v>
+      </c>
+      <c r="J286" s="14">
+        <f>H286/G286</f>
+        <v>1.3193012180674841E-3</v>
+      </c>
+      <c r="K286" s="19">
+        <f>J286</f>
+        <v>1.3193012180674841E-3</v>
+      </c>
+      <c r="L286" s="15">
+        <f>MIN(D286:D287)</f>
+        <v>8.1364901690717204</v>
+      </c>
+      <c r="M286" s="15">
+        <f>MAX(D286:D287)</f>
+        <v>8.1516851934779702</v>
+      </c>
+      <c r="N286" s="14">
+        <f>M286-L286</f>
+        <v>1.5195024406249757E-2</v>
+      </c>
+    </row>
+    <row r="287" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A287" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="B287" s="18">
+        <v>44314</v>
+      </c>
+      <c r="D287" s="15">
+        <v>8.1364901690717204</v>
+      </c>
+      <c r="E287" s="15">
+        <v>8.0156626767209094</v>
+      </c>
+      <c r="F287" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="288" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A288" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="B288" s="18">
+        <v>44314</v>
+      </c>
+      <c r="D288" s="15">
+        <v>7.9415588714037204</v>
+      </c>
+      <c r="E288" s="15">
+        <v>7.8149377237633297</v>
+      </c>
+      <c r="F288" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G288" s="15">
+        <f>AVERAGE(D288:D289)</f>
+        <v>7.9473683666312755</v>
+      </c>
+      <c r="H288" s="14">
+        <f>_xlfn.STDEV.S(D288:D289)</f>
+        <v>8.2158669413496203E-3</v>
+      </c>
+      <c r="I288" s="14">
+        <f>2*H288</f>
+        <v>1.6431733882699241E-2</v>
+      </c>
+      <c r="J288" s="14">
+        <f>H288/G288</f>
+        <v>1.0337845891031921E-3</v>
+      </c>
+      <c r="K288" s="19">
+        <f>J288</f>
+        <v>1.0337845891031921E-3</v>
+      </c>
+      <c r="L288" s="15">
+        <f>MIN(D288:D289)</f>
+        <v>7.9415588714037204</v>
+      </c>
+      <c r="M288" s="15">
+        <f>MAX(D288:D289)</f>
+        <v>7.9531778618588298</v>
+      </c>
+      <c r="N288" s="14">
+        <f>M288-L288</f>
+        <v>1.161899045510939E-2</v>
+      </c>
+    </row>
+    <row r="289" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A289" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="B289" s="18">
+        <v>44314</v>
+      </c>
+      <c r="D289" s="15">
+        <v>7.9531778618588298</v>
+      </c>
+      <c r="E289" s="15">
+        <v>7.8268542046040803</v>
+      </c>
+      <c r="F289" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="290" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A290" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="B290" s="18">
+        <v>44321</v>
+      </c>
+      <c r="D290" s="15">
+        <v>8.0121510421289202</v>
+      </c>
+      <c r="E290" s="15">
+        <v>7.8537609950039702</v>
+      </c>
+    </row>
+    <row r="291" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A291" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="B291" s="18">
+        <v>44321</v>
+      </c>
+      <c r="D291" s="15">
+        <v>8.1192616644881497</v>
+      </c>
+      <c r="E291" s="15">
+        <v>8.0006583506477202</v>
+      </c>
+      <c r="F291" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G291" s="15">
+        <f>AVERAGE(D291:D292)</f>
+        <v>8.1205856668101539</v>
+      </c>
+      <c r="H291" s="14">
+        <f>_xlfn.STDEV.S(D291:D292)</f>
+        <v>1.8724220403931325E-3</v>
+      </c>
+      <c r="I291" s="14">
+        <f>2*H291</f>
+        <v>3.744844080786265E-3</v>
+      </c>
+      <c r="J291" s="14">
+        <f>H291/G291</f>
+        <v>2.3057721662194327E-4</v>
+      </c>
+      <c r="K291" s="19">
+        <f>J291</f>
+        <v>2.3057721662194327E-4</v>
+      </c>
+      <c r="L291" s="15">
+        <f>MIN(D291:D292)</f>
+        <v>8.1192616644881497</v>
+      </c>
+      <c r="M291" s="15">
+        <f>MAX(D291:D292)</f>
+        <v>8.1219096691321599</v>
+      </c>
+      <c r="N291" s="14">
+        <f>M291-L291</f>
+        <v>2.6480046440102711E-3</v>
+      </c>
+    </row>
+    <row r="292" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A292" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="B292" s="18">
+        <v>44321</v>
+      </c>
+      <c r="D292" s="15">
+        <v>8.1219096691321599</v>
+      </c>
+      <c r="E292" s="15">
+        <v>8.0038990809154598</v>
+      </c>
+      <c r="F292" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="293" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A293" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="B293" s="18">
+        <v>44321</v>
+      </c>
+      <c r="D293" s="15">
+        <v>7.9968868002810796</v>
+      </c>
+      <c r="E293" s="15">
+        <v>7.8677353231236404</v>
+      </c>
+      <c r="F293" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G293" s="15">
+        <f>AVERAGE(D293:D294)</f>
+        <v>7.9964727794401504</v>
+      </c>
+      <c r="H293" s="14">
+        <f>_xlfn.STDEV.S(D293:D294)</f>
+        <v>5.85513888347702E-4</v>
+      </c>
+      <c r="I293" s="14">
+        <f>2*H293</f>
+        <v>1.171027776695404E-3</v>
+      </c>
+      <c r="J293" s="14">
+        <f>H293/G293</f>
+        <v>7.3221519599632156E-5</v>
+      </c>
+      <c r="K293" s="19">
+        <f>J293</f>
+        <v>7.3221519599632156E-5</v>
+      </c>
+      <c r="L293" s="15">
+        <f>MIN(D293:D294)</f>
+        <v>7.9960587585992204</v>
+      </c>
+      <c r="M293" s="15">
+        <f>MAX(D293:D294)</f>
+        <v>7.9968868002810796</v>
+      </c>
+      <c r="N293" s="14">
+        <f>M293-L293</f>
+        <v>8.280416818591263E-4</v>
+      </c>
+    </row>
+    <row r="294" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A294" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="B294" s="18">
+        <v>44321</v>
+      </c>
+      <c r="D294" s="15">
+        <v>7.9960587585992204</v>
+      </c>
+      <c r="E294" s="15">
+        <v>7.8669072814417804</v>
+      </c>
+      <c r="F294" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="295" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A295" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="B295" s="18">
+        <v>44321</v>
+      </c>
+      <c r="D295" s="15">
+        <v>8.0003142176561095</v>
+      </c>
+      <c r="E295" s="15">
+        <v>7.8711627404986597</v>
+      </c>
+      <c r="F295" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G295" s="15">
+        <f>AVERAGE(D295:D296)</f>
+        <v>8.0003832741505452</v>
+      </c>
+      <c r="H295" s="14">
+        <f>_xlfn.STDEV.S(D295:D296)</f>
+        <v>9.76606310008679E-5</v>
+      </c>
+      <c r="I295" s="14">
+        <f>2*H295</f>
+        <v>1.953212620017358E-4</v>
+      </c>
+      <c r="J295" s="14">
+        <f>H295/G295</f>
+        <v>1.2206994046949231E-5</v>
+      </c>
+      <c r="K295" s="19">
+        <f>J295</f>
+        <v>1.2206994046949231E-5</v>
+      </c>
+      <c r="L295" s="15">
+        <f>MIN(D295:D296)</f>
+        <v>8.0003142176561095</v>
+      </c>
+      <c r="M295" s="15">
+        <f>MAX(D295:D296)</f>
+        <v>8.0004523306449808</v>
+      </c>
+      <c r="N295" s="14">
+        <f>M295-L295</f>
+        <v>1.3811298887134171E-4</v>
+      </c>
+    </row>
+    <row r="296" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A296" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="B296" s="18">
+        <v>44321</v>
+      </c>
+      <c r="D296" s="15">
+        <v>8.0004523306449808</v>
+      </c>
+      <c r="E296" s="15">
+        <v>7.8713008534875399</v>
+      </c>
+      <c r="F296" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="297" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A297" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="B297" s="18">
+        <v>44321</v>
+      </c>
+      <c r="D297" s="15">
+        <v>7.7430536654415096</v>
+      </c>
+      <c r="E297" s="15">
+        <v>7.6130084204383799</v>
+      </c>
+      <c r="F297" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G297" s="15">
+        <f>AVERAGE(D297:D298)</f>
+        <v>7.7399035682712292</v>
+      </c>
+      <c r="H297" s="14">
+        <f>_xlfn.STDEV.S(D297:D298)</f>
+        <v>4.4549101410031279E-3</v>
+      </c>
+      <c r="I297" s="14">
+        <f>2*H297</f>
+        <v>8.9098202820062557E-3</v>
+      </c>
+      <c r="J297" s="14">
+        <f>H297/G297</f>
+        <v>5.7557695670337251E-4</v>
+      </c>
+      <c r="K297" s="19">
+        <f>J297</f>
+        <v>5.7557695670337251E-4</v>
+      </c>
+      <c r="L297" s="15">
+        <f>MIN(D297:D298)</f>
+        <v>7.7367534711009496</v>
+      </c>
+      <c r="M297" s="15">
+        <f>MAX(D297:D298)</f>
+        <v>7.7430536654415096</v>
+      </c>
+      <c r="N297" s="14">
+        <f>M297-L297</f>
+        <v>6.3001943405600613E-3</v>
+      </c>
+    </row>
+    <row r="298" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A298" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="B298" s="18">
+        <v>44321</v>
+      </c>
+      <c r="D298" s="15">
+        <v>7.7367534711009496</v>
+      </c>
+      <c r="E298" s="15">
+        <v>7.6067082260978198</v>
+      </c>
+      <c r="F298" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="299" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A299" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="B299" s="18">
+        <v>44328</v>
+      </c>
+      <c r="D299" s="15">
+        <v>7.9896302680363904</v>
+      </c>
+      <c r="E299" s="15">
+        <v>7.8312402209114502</v>
+      </c>
+    </row>
+    <row r="300" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="B300" s="18">
+        <v>44328</v>
+      </c>
+      <c r="D300" s="15">
+        <v>7.88213110895299</v>
+      </c>
+      <c r="E300" s="15">
+        <v>7.7520858639498602</v>
+      </c>
+      <c r="F300" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G300" s="15">
+        <f>AVERAGE(D300:D301)</f>
+        <v>7.8813492661007896</v>
+      </c>
+      <c r="H300" s="14">
+        <f>_xlfn.STDEV.S(D300:D301)</f>
+        <v>1.1056927652256386E-3</v>
+      </c>
+      <c r="I300" s="14">
+        <f>2*H300</f>
+        <v>2.2113855304512773E-3</v>
+      </c>
+      <c r="J300" s="14">
+        <f>H300/G300</f>
+        <v>1.4029231897911662E-4</v>
+      </c>
+      <c r="K300" s="19">
+        <f>J300</f>
+        <v>1.4029231897911662E-4</v>
+      </c>
+      <c r="L300" s="15">
+        <f>MIN(D300:D301)</f>
+        <v>7.8805674232485901</v>
+      </c>
+      <c r="M300" s="15">
+        <f>MAX(D300:D301)</f>
+        <v>7.88213110895299</v>
+      </c>
+      <c r="N300" s="14">
+        <f>M300-L300</f>
+        <v>1.5636857043999086E-3</v>
+      </c>
+    </row>
+    <row r="301" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A301" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="B301" s="18">
+        <v>44328</v>
+      </c>
+      <c r="D301" s="15">
+        <v>7.8805674232485901</v>
+      </c>
+      <c r="E301" s="15">
+        <v>7.7505221782454603</v>
+      </c>
+      <c r="F301" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="302" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A302" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="B302" s="18">
+        <v>44328</v>
+      </c>
+      <c r="D302" s="15">
+        <v>8.2615768527577291</v>
+      </c>
+      <c r="E302" s="15">
+        <v>8.1435662645410201</v>
+      </c>
+      <c r="F302" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G302" s="15">
+        <f>AVERAGE(D302:D303)</f>
+        <v>8.2624708831349203</v>
+      </c>
+      <c r="H302" s="14">
+        <f>_xlfn.STDEV.S(D302:D303)</f>
+        <v>1.2643498845960124E-3</v>
+      </c>
+      <c r="I302" s="14">
+        <f>2*H302</f>
+        <v>2.5286997691920249E-3</v>
+      </c>
+      <c r="J302" s="14">
+        <f>H302/G302</f>
+        <v>1.5302321817275765E-4</v>
+      </c>
+      <c r="K302" s="19">
+        <f>J302</f>
+        <v>1.5302321817275765E-4</v>
+      </c>
+      <c r="L302" s="15">
+        <f>MIN(D302:D303)</f>
+        <v>8.2615768527577291</v>
+      </c>
+      <c r="M302" s="15">
+        <f>MAX(D302:D303)</f>
+        <v>8.2633649135121097</v>
+      </c>
+      <c r="N302" s="14">
+        <f>M302-L302</f>
+        <v>1.7880607543805382E-3</v>
+      </c>
+    </row>
+    <row r="303" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A303" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="B303" s="18">
+        <v>44328</v>
+      </c>
+      <c r="D303" s="15">
+        <v>8.2633649135121097</v>
+      </c>
+      <c r="E303" s="15">
+        <v>8.1453543252954006</v>
+      </c>
+      <c r="F303" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="304" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A304" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="B304" s="18">
+        <v>44328</v>
+      </c>
+      <c r="D304" s="15">
+        <v>8.1205899603182896</v>
+      </c>
+      <c r="E304" s="15">
+        <v>8.0274734824806</v>
+      </c>
+      <c r="F304" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G304" s="15">
+        <f>AVERAGE(D304:D305)</f>
+        <v>8.1166018939598299</v>
+      </c>
+      <c r="H304" s="14">
+        <f>_xlfn.STDEV.S(D304:D305)</f>
+        <v>5.6399775317776159E-3</v>
+      </c>
+      <c r="I304" s="14">
+        <f>2*H304</f>
+        <v>1.1279955063555232E-2</v>
+      </c>
+      <c r="J304" s="14">
+        <f>H304/G304</f>
+        <v>6.9486930681850298E-4</v>
+      </c>
+      <c r="K304" s="19">
+        <f>J304</f>
+        <v>6.9486930681850298E-4</v>
+      </c>
+      <c r="L304" s="15">
+        <f>MIN(D304:D305)</f>
+        <v>8.1126138276013702</v>
+      </c>
+      <c r="M304" s="15">
+        <f>MAX(D304:D305)</f>
+        <v>8.1205899603182896</v>
+      </c>
+      <c r="N304" s="14">
+        <f>M304-L304</f>
+        <v>7.9761327169194374E-3</v>
+      </c>
+    </row>
+    <row r="305" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A305" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="B305" s="18">
+        <v>44328</v>
+      </c>
+      <c r="D305" s="15">
+        <v>8.1126138276013702</v>
+      </c>
+      <c r="E305" s="15">
+        <v>8.0194973497636806</v>
+      </c>
+      <c r="F305" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="306" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A306" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="B306" s="18">
+        <v>44328</v>
+      </c>
+      <c r="D306" s="15">
+        <v>7.9362787138669502</v>
+      </c>
+      <c r="E306" s="15">
+        <v>7.8440407484992596</v>
+      </c>
+      <c r="F306" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G306" s="15">
+        <f>AVERAGE(D306:D307)</f>
+        <v>7.9379263397158795</v>
+      </c>
+      <c r="H306" s="14">
+        <f>_xlfn.STDEV.S(D306:D307)</f>
+        <v>2.3300948212729307E-3</v>
+      </c>
+      <c r="I306" s="14">
+        <f>2*H306</f>
+        <v>4.6601896425458615E-3</v>
+      </c>
+      <c r="J306" s="14">
+        <f>H306/G306</f>
+        <v>2.9353948645438442E-4</v>
+      </c>
+      <c r="K306" s="19">
+        <f>J306</f>
+        <v>2.9353948645438442E-4</v>
+      </c>
+      <c r="L306" s="15">
+        <f>MIN(D306:D307)</f>
+        <v>7.9362787138669502</v>
+      </c>
+      <c r="M306" s="15">
+        <f>MAX(D306:D307)</f>
+        <v>7.9395739655648097</v>
+      </c>
+      <c r="N306" s="14">
+        <f>M306-L306</f>
+        <v>3.2952516978594915E-3</v>
+      </c>
+    </row>
+    <row r="307" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A307" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="B307" s="18">
+        <v>44328</v>
+      </c>
+      <c r="D307" s="15">
+        <v>7.9395739655648097</v>
+      </c>
+      <c r="E307" s="15">
+        <v>7.8473360001971102</v>
+      </c>
+      <c r="F307" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="308" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A308" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="B308" s="18">
+        <v>44335</v>
+      </c>
+      <c r="D308" s="15">
+        <v>7.9975723607825104</v>
+      </c>
+      <c r="E308" s="15">
+        <v>7.8391823136575702</v>
+      </c>
+    </row>
+    <row r="309" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A309" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="B309" s="18">
+        <v>44335</v>
+      </c>
+      <c r="D309" s="15">
+        <v>8.0569542779642394</v>
+      </c>
+      <c r="E309" s="15">
+        <v>7.9152562057514002</v>
+      </c>
+      <c r="F309" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G309" s="15">
+        <f>AVERAGE(D309:D310)</f>
+        <v>8.0531794343566894</v>
+      </c>
+      <c r="H309" s="14">
+        <f>_xlfn.STDEV.S(D309:D310)</f>
+        <v>5.3384350256345664E-3</v>
+      </c>
+      <c r="I309" s="14">
+        <f>2*H309</f>
+        <v>1.0676870051269133E-2</v>
+      </c>
+      <c r="J309" s="14">
+        <f>H309/G309</f>
+        <v>6.6289781187037656E-4</v>
+      </c>
+      <c r="K309" s="19">
+        <f>J309</f>
+        <v>6.6289781187037656E-4</v>
+      </c>
+      <c r="L309" s="15">
+        <f>MIN(D309:D310)</f>
+        <v>8.0494045907491394</v>
+      </c>
+      <c r="M309" s="15">
+        <f>MAX(D309:D310)</f>
+        <v>8.0569542779642394</v>
+      </c>
+      <c r="N309" s="14">
+        <f>M309-L309</f>
+        <v>7.549687215099965E-3</v>
+      </c>
+    </row>
+    <row r="310" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A310" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="B310" s="18">
+        <v>44335</v>
+      </c>
+      <c r="D310" s="15">
+        <v>8.0494045907491394</v>
+      </c>
+      <c r="E310" s="15">
+        <v>7.90815586972957</v>
+      </c>
+      <c r="F310" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="311" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A311" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="B311" s="18">
+        <v>44335</v>
+      </c>
+      <c r="D311" s="15">
+        <v>7.9120235208493197</v>
+      </c>
+      <c r="E311" s="15">
+        <v>7.7776531637036896</v>
+      </c>
+      <c r="F311" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G311" s="15">
+        <f>AVERAGE(D311:D312)</f>
+        <v>7.9096357864778852</v>
+      </c>
+      <c r="H311" s="14">
+        <f>_xlfn.STDEV.S(D311:D312)</f>
+        <v>3.3767663314276512E-3</v>
+      </c>
+      <c r="I311" s="14">
+        <f>2*H311</f>
+        <v>6.7535326628553024E-3</v>
+      </c>
+      <c r="J311" s="14">
+        <f>H311/G311</f>
+        <v>4.2691805572141336E-4</v>
+      </c>
+      <c r="K311" s="19">
+        <f>J311</f>
+        <v>4.2691805572141336E-4</v>
+      </c>
+      <c r="L311" s="15">
+        <f>MIN(D311:D312)</f>
+        <v>7.9072480521064499</v>
+      </c>
+      <c r="M311" s="15">
+        <f>MAX(D311:D312)</f>
+        <v>7.9120235208493197</v>
+      </c>
+      <c r="N311" s="14">
+        <f>M311-L311</f>
+        <v>4.7754687428698261E-3</v>
+      </c>
+    </row>
+    <row r="312" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A312" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="B312" s="18">
+        <v>44335</v>
+      </c>
+      <c r="D312" s="15">
+        <v>7.9072480521064499</v>
+      </c>
+      <c r="E312" s="15">
+        <v>7.7730269813211104</v>
+      </c>
+      <c r="F312" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="313" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A313" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="B313" s="18">
+        <v>44335</v>
+      </c>
+      <c r="D313" s="15">
+        <v>8.1040814680389701</v>
+      </c>
+      <c r="E313" s="15">
+        <v>7.9629825099767801</v>
+      </c>
+      <c r="F313" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G313" s="15">
+        <f>AVERAGE(D313:D314)</f>
+        <v>8.1049547225277863</v>
+      </c>
+      <c r="H313" s="14">
+        <f>_xlfn.STDEV.S(D313:D314)</f>
+        <v>1.2349683414857194E-3</v>
+      </c>
+      <c r="I313" s="14">
+        <f>2*H313</f>
+        <v>2.4699366829714388E-3</v>
+      </c>
+      <c r="J313" s="14">
+        <f>H313/G313</f>
+        <v>1.5237202227090979E-4</v>
+      </c>
+      <c r="K313" s="19">
+        <f>J313</f>
+        <v>1.5237202227090979E-4</v>
+      </c>
+      <c r="L313" s="15">
+        <f>MIN(D313:D314)</f>
+        <v>8.1040814680389701</v>
+      </c>
+      <c r="M313" s="15">
+        <f>MAX(D313:D314)</f>
+        <v>8.1058279770166006</v>
+      </c>
+      <c r="N313" s="14">
+        <f>M313-L313</f>
+        <v>1.746508977630512E-3</v>
+      </c>
+    </row>
+    <row r="314" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A314" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="B314" s="18">
+        <v>44335</v>
+      </c>
+      <c r="D314" s="15">
+        <v>8.1058279770166006</v>
+      </c>
+      <c r="E314" s="15">
+        <v>7.9650285137150503</v>
+      </c>
+      <c r="F314" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="315" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A315" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="B315" s="18">
+        <v>44335</v>
+      </c>
+      <c r="D315" s="15">
+        <v>7.8624295802646396</v>
+      </c>
+      <c r="E315" s="15">
+        <v>7.76726183362159</v>
+      </c>
+      <c r="F315" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G315" s="15">
+        <f>AVERAGE(D315:D316)</f>
+        <v>7.8554343182364352</v>
+      </c>
+      <c r="H315" s="14">
+        <f>_xlfn.STDEV.S(D315:D316)</f>
+        <v>9.8927944326407148E-3</v>
+      </c>
+      <c r="I315" s="14">
+        <f>2*H315</f>
+        <v>1.978558886528143E-2</v>
+      </c>
+      <c r="J315" s="14">
+        <f>H315/G315</f>
+        <v>1.2593567754330957E-3</v>
+      </c>
+      <c r="K315" s="19">
+        <f>J315</f>
+        <v>1.2593567754330957E-3</v>
+      </c>
+      <c r="L315" s="15">
+        <f>MIN(D315:D316)</f>
+        <v>7.84843905620823</v>
+      </c>
+      <c r="M315" s="15">
+        <f>MAX(D315:D316)</f>
+        <v>7.8624295802646396</v>
+      </c>
+      <c r="N315" s="14">
+        <f>M315-L315</f>
+        <v>1.3990524056409548E-2</v>
+      </c>
+    </row>
+    <row r="316" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A316" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="B316" s="18">
+        <v>44335</v>
+      </c>
+      <c r="D316" s="15">
+        <v>7.84843905620823</v>
+      </c>
+      <c r="E316" s="15">
+        <v>7.7525382359909099</v>
+      </c>
+      <c r="F316" s="16" t="s">
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -9548,7 +11047,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Imported Christian's latest pH data and updated the compiled Nielsen Lab and Christian's sample excel spreadsheets
</commit_message>
<xml_diff>
--- a/check sample work/pH QAQC/20210326 pH check sample results summary.xlsx
+++ b/check sample work/pH QAQC/20210326 pH check sample results summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rye-Tech\Documents\R\rye-tech-home\2021-season-summary\check sample work\pH QAQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96CA47B-E28A-49A9-802E-EFB50DF5BD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C912306E-A42F-4AC6-976D-E6A45817D0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="example to follow" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="381">
   <si>
     <t>sample</t>
   </si>
@@ -1168,6 +1168,12 @@
   </si>
   <si>
     <t xml:space="preserve"> T21-708-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T21-714-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T21-714-2</t>
   </si>
 </sst>
 </file>
@@ -1849,20 +1855,20 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="13" max="13" width="51.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" customWidth="1"/>
+    <col min="13" max="13" width="51.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1900,7 +1906,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1914,7 +1920,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1925,7 +1931,7 @@
         <v>2247.5363699999998</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1969,7 +1975,7 @@
       </c>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1980,7 +1986,7 @@
         <v>2114.1481899999999</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1991,7 +1997,7 @@
         <v>2138.9193500000001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2035,7 +2041,7 @@
       </c>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2046,7 +2052,7 @@
         <v>2135.2389699999999</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2057,7 +2063,7 @@
         <v>2133.48756</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2101,7 +2107,7 @@
       </c>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2112,7 +2118,7 @@
         <v>2124.9360900000001</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2123,7 +2129,7 @@
         <v>2132.3921700000001</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2167,7 +2173,7 @@
       </c>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2178,7 +2184,7 @@
         <v>2249.3508299999999</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -2189,7 +2195,7 @@
         <v>2250.2915600000001</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2236,10 +2242,10 @@
       </c>
       <c r="M16" s="3"/>
     </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:14" x14ac:dyDescent="0.3">
       <c r="N20" s="4"/>
     </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
         <v>34</v>
       </c>
@@ -2250,7 +2256,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E22">
         <f>2238.04</f>
         <v>2238.04</v>
@@ -2264,7 +2270,7 @@
         <v>21.704231088401922</v>
       </c>
     </row>
-    <row r="23" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E23">
         <f t="shared" ref="E23:E26" si="0">2238.04</f>
         <v>2238.04</v>
@@ -2278,7 +2284,7 @@
         <v>90.181043176897006</v>
       </c>
     </row>
-    <row r="24" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E24">
         <f t="shared" si="0"/>
         <v>2238.04</v>
@@ -2292,7 +2298,7 @@
         <v>62.986127504401573</v>
       </c>
     </row>
-    <row r="25" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E25">
         <f>2238.04</f>
         <v>2238.04</v>
@@ -2306,7 +2312,7 @@
         <v>127.93487528889766</v>
       </c>
     </row>
-    <row r="26" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E26">
         <f t="shared" si="0"/>
         <v>2238.04</v>
@@ -2320,7 +2326,7 @@
         <v>150.10072243360378</v>
       </c>
     </row>
-    <row r="29" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:14" x14ac:dyDescent="0.3">
       <c r="G29">
         <f>SQRT(SUM(G22:G26)/5)</f>
         <v>9.5174261173092578</v>
@@ -2329,7 +2335,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:14" x14ac:dyDescent="0.3">
       <c r="F30" s="3"/>
       <c r="G30">
         <v>0.53</v>
@@ -2338,7 +2344,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:14" x14ac:dyDescent="0.3">
       <c r="G31">
         <f>SQRT(G29^2+G30^2)</f>
         <v>9.5321718353395397</v>
@@ -2350,7 +2356,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:14" x14ac:dyDescent="0.3">
       <c r="G32">
         <f>G31/E26</f>
         <v>4.2591606206053246E-3</v>
@@ -2362,12 +2368,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:13" x14ac:dyDescent="0.3">
       <c r="M36" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="4:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D37" s="1" t="s">
         <v>38</v>
       </c>
@@ -2380,29 +2386,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O316"/>
+  <dimension ref="A1:O319"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O304" sqref="O304"/>
+      <pane ySplit="1" topLeftCell="A307" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D325" sqref="D325"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.88671875" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="13" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="14" customWidth="1"/>
     <col min="11" max="14" width="13" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="51.140625" style="17" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="17"/>
+    <col min="15" max="15" width="51.109375" style="17" customWidth="1"/>
+    <col min="16" max="16384" width="9.109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2446,7 +2452,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>50</v>
       </c>
@@ -2461,7 +2467,7 @@
         <v>7.74153486291614</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>51</v>
       </c>
@@ -2508,7 +2514,7 @@
         <v>9.4507647610004852E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>52</v>
       </c>
@@ -2529,7 +2535,7 @@
       <c r="K4" s="19"/>
       <c r="O4" s="20"/>
     </row>
-    <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>53</v>
       </c>
@@ -2543,7 +2549,7 @@
         <v>8.0789632362488106</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>55</v>
       </c>
@@ -2589,7 +2595,7 @@
         <v>1.6392079000000059E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>56</v>
       </c>
@@ -2603,7 +2609,7 @@
         <v>7.8272875099999997</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>57</v>
       </c>
@@ -2623,7 +2629,7 @@
       <c r="K8" s="19"/>
       <c r="O8" s="20"/>
     </row>
-    <row r="9" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>58</v>
       </c>
@@ -2643,7 +2649,7 @@
       <c r="K9" s="19"/>
       <c r="O9" s="20"/>
     </row>
-    <row r="10" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>59</v>
       </c>
@@ -2663,7 +2669,7 @@
       <c r="K10" s="19"/>
       <c r="O10" s="20"/>
     </row>
-    <row r="11" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>60</v>
       </c>
@@ -2683,7 +2689,7 @@
       <c r="K11" s="19"/>
       <c r="O11" s="20"/>
     </row>
-    <row r="12" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>61</v>
       </c>
@@ -2703,7 +2709,7 @@
       <c r="K12" s="19"/>
       <c r="O12" s="20"/>
     </row>
-    <row r="13" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>62</v>
       </c>
@@ -2750,7 +2756,7 @@
       </c>
       <c r="O13" s="20"/>
     </row>
-    <row r="14" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>63</v>
       </c>
@@ -2770,7 +2776,7 @@
       <c r="K14" s="19"/>
       <c r="O14" s="20"/>
     </row>
-    <row r="15" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>64</v>
       </c>
@@ -2790,7 +2796,7 @@
       <c r="K15" s="19"/>
       <c r="O15" s="20"/>
     </row>
-    <row r="16" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>65</v>
       </c>
@@ -2810,7 +2816,7 @@
       <c r="K16" s="19"/>
       <c r="O16" s="20"/>
     </row>
-    <row r="17" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>66</v>
       </c>
@@ -2824,7 +2830,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>67</v>
       </c>
@@ -2838,7 +2844,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>68</v>
       </c>
@@ -2852,7 +2858,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>69</v>
       </c>
@@ -2866,7 +2872,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>70</v>
       </c>
@@ -2880,7 +2886,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
         <v>71</v>
       </c>
@@ -2926,7 +2932,7 @@
         <v>5.8186829255406636E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
         <v>72</v>
       </c>
@@ -2940,7 +2946,7 @@
         <v>7.7988739523662698</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
         <v>73</v>
       </c>
@@ -2954,7 +2960,7 @@
         <v>7.79305526944073</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
         <v>74</v>
       </c>
@@ -3000,7 +3006,7 @@
         <v>8.4581219180899225E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
         <v>75</v>
       </c>
@@ -3014,7 +3020,7 @@
         <v>7.9540741754416899</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
         <v>76</v>
       </c>
@@ -3028,7 +3034,7 @@
         <v>7.9594204270895696</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
         <v>77</v>
       </c>
@@ -3042,7 +3048,7 @@
         <v>8.0873331962983404</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
         <v>78</v>
       </c>
@@ -3088,7 +3094,7 @@
         <v>1.3818509232670806E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
         <v>79</v>
       </c>
@@ -3102,7 +3108,7 @@
         <v>7.9935739879872703</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
         <v>80</v>
       </c>
@@ -3116,7 +3122,7 @@
         <v>7.9966718658117797</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
         <v>81</v>
       </c>
@@ -3162,7 +3168,7 @@
         <v>2.2264576316979756E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>82</v>
       </c>
@@ -3176,7 +3182,7 @@
         <v>7.8397113904705504</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
         <v>83</v>
       </c>
@@ -3190,7 +3196,7 @@
         <v>7.8274796640885898</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
         <v>44</v>
       </c>
@@ -3237,7 +3243,7 @@
         <v>4.9836338999999619E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
         <v>45</v>
       </c>
@@ -3252,7 +3258,7 @@
         <v>7.6206292969999998</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
         <v>46</v>
       </c>
@@ -3273,7 +3279,7 @@
       <c r="K37" s="19"/>
       <c r="O37" s="20"/>
     </row>
-    <row r="38" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="14" t="s">
         <v>84</v>
       </c>
@@ -3319,7 +3325,7 @@
         <v>1.0153592664430278E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
         <v>85</v>
       </c>
@@ -3333,7 +3339,7 @@
         <v>7.6916903045289899</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
         <v>86</v>
       </c>
@@ -3347,7 +3353,7 @@
         <v>7.69283522006263</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="14" t="s">
         <v>44</v>
       </c>
@@ -3393,7 +3399,7 @@
         <v>4.9682060142279383E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
         <v>45</v>
       </c>
@@ -3407,7 +3413,7 @@
         <v>7.6206853918415103</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
         <v>46</v>
       </c>
@@ -3421,7 +3427,7 @@
         <v>7.5723148968455796</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="14" t="s">
         <v>87</v>
       </c>
@@ -3467,7 +3473,7 @@
         <v>6.4461798622197364E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="14" t="s">
         <v>88</v>
       </c>
@@ -3481,7 +3487,7 @@
         <v>7.7435457498339</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
         <v>89</v>
       </c>
@@ -3495,7 +3501,7 @@
         <v>7.7425531075232099</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="s">
         <v>90</v>
       </c>
@@ -3541,7 +3547,7 @@
         <v>1.9858913499604114E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
         <v>91</v>
       </c>
@@ -3555,7 +3561,7 @@
         <v>7.85309992140568</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
         <v>92</v>
       </c>
@@ -3569,7 +3575,7 @@
         <v>7.8511140300557098</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
         <v>93</v>
       </c>
@@ -3583,7 +3589,7 @@
         <v>7.6858002409995496</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
         <v>94</v>
       </c>
@@ -3597,7 +3603,7 @@
         <v>7.6604061490644897</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="14" t="s">
         <v>95</v>
       </c>
@@ -3611,7 +3617,7 @@
         <v>8.0900620266582006</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="14" t="s">
         <v>96</v>
       </c>
@@ -3625,7 +3631,7 @@
         <v>7.6378195889536498</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="14" t="s">
         <v>97</v>
       </c>
@@ -3639,7 +3645,7 @@
         <v>7.6496254781234603</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="14" t="s">
         <v>98</v>
       </c>
@@ -3653,7 +3659,7 @@
         <v>8.0839369011466005</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="14" t="s">
         <v>99</v>
       </c>
@@ -3699,7 +3705,7 @@
         <v>1.9675741874287667E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="14" t="s">
         <v>100</v>
       </c>
@@ -3713,7 +3719,7 @@
         <v>7.8860289201581297</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="14" t="s">
         <v>101</v>
       </c>
@@ -3727,7 +3733,7 @@
         <v>7.8842376073644704</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="14" t="s">
         <v>102</v>
       </c>
@@ -3741,7 +3747,7 @@
         <v>8.0814347249955993</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="14" t="s">
         <v>144</v>
       </c>
@@ -3762,7 +3768,7 @@
       <c r="L60" s="15"/>
       <c r="M60" s="15"/>
     </row>
-    <row r="61" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="14" t="s">
         <v>145</v>
       </c>
@@ -3779,7 +3785,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="14" t="s">
         <v>146</v>
       </c>
@@ -3796,7 +3802,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="14" t="s">
         <v>131</v>
       </c>
@@ -3813,7 +3819,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="14" t="s">
         <v>132</v>
       </c>
@@ -3830,7 +3836,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="14" t="s">
         <v>133</v>
       </c>
@@ -3847,7 +3853,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="14" t="s">
         <v>134</v>
       </c>
@@ -3864,7 +3870,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="14" t="s">
         <v>135</v>
       </c>
@@ -3881,7 +3887,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="14" t="s">
         <v>136</v>
       </c>
@@ -3898,7 +3904,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="14" t="s">
         <v>123</v>
       </c>
@@ -3944,7 +3950,7 @@
         <v>3.9238010000000045E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="14" t="s">
         <v>124</v>
       </c>
@@ -3958,7 +3964,7 @@
         <v>7.7374005620000004</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="14" t="s">
         <v>125</v>
       </c>
@@ -3972,7 +3978,7 @@
         <v>7.7393420920000002</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="14" t="s">
         <v>126</v>
       </c>
@@ -3986,7 +3992,7 @@
         <v>7.7354182920000003</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="14" t="s">
         <v>127</v>
       </c>
@@ -4032,7 +4038,7 @@
         <v>0.16391599100000054</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="14" t="s">
         <v>128</v>
       </c>
@@ -4046,7 +4052,7 @@
         <v>7.0702561770000001</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="14" t="s">
         <v>129</v>
       </c>
@@ -4060,7 +4066,7 @@
         <v>7.0495923649999996</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="14" t="s">
         <v>130</v>
       </c>
@@ -4074,7 +4080,7 @@
         <v>8.0626476389999997</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="14" t="s">
         <v>117</v>
       </c>
@@ -4120,7 +4126,7 @@
         <v>1.9808850000000433E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="14" t="s">
         <v>118</v>
       </c>
@@ -4134,7 +4140,7 @@
         <v>7.2533112170000003</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="14" t="s">
         <v>119</v>
       </c>
@@ -4148,7 +4154,7 @@
         <v>7.2335023679999999</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="14" t="s">
         <v>120</v>
       </c>
@@ -4194,7 +4200,7 @@
         <v>5.2714730000005261E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="14" t="s">
         <v>121</v>
       </c>
@@ -4208,7 +4214,7 @@
         <v>7.774027029</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="14" t="s">
         <v>122</v>
       </c>
@@ -4222,7 +4228,7 @@
         <v>7.7718314790000003</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="14" t="s">
         <v>113</v>
       </c>
@@ -4268,7 +4274,7 @@
         <v>5.5175080000005039E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="14" t="s">
         <v>114</v>
       </c>
@@ -4282,7 +4288,7 @@
         <v>7.7390057639999998</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="14" t="s">
         <v>115</v>
       </c>
@@ -4328,7 +4334,7 @@
         <v>0.39663596199999951</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="14" t="s">
         <v>116</v>
       </c>
@@ -4342,7 +4348,7 @@
         <v>6.3836745009999998</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="14" t="s">
         <v>137</v>
       </c>
@@ -4388,7 +4394,7 @@
         <v>3.3557309999991958E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="14" t="s">
         <v>138</v>
       </c>
@@ -4402,7 +4408,7 @@
         <v>7.8138157469999996</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="14" t="s">
         <v>139</v>
       </c>
@@ -4448,7 +4454,7 @@
         <v>3.984354099999976E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="14" t="s">
         <v>140</v>
       </c>
@@ -4462,7 +4468,7 @@
         <v>7.1890400999999997</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="14" t="s">
         <v>141</v>
       </c>
@@ -4508,7 +4514,7 @@
         <v>1.0579034000000043E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="14" t="s">
         <v>142</v>
       </c>
@@ -4522,7 +4528,7 @@
         <v>7.8047359729999997</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="14" t="s">
         <v>143</v>
       </c>
@@ -4536,7 +4542,7 @@
         <v>7.7955808449999999</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="14" t="s">
         <v>103</v>
       </c>
@@ -4582,7 +4588,7 @@
         <v>1.0066078000000367E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="14" t="s">
         <v>104</v>
       </c>
@@ -4596,7 +4602,7 @@
         <v>7.8017914089999998</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="14" t="s">
         <v>105</v>
       </c>
@@ -4610,7 +4616,7 @@
         <v>7.8118574880000002</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="14" t="s">
         <v>106</v>
       </c>
@@ -4656,7 +4662,7 @@
         <v>1.5797846999999976E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="14" t="s">
         <v>107</v>
       </c>
@@ -4670,7 +4676,7 @@
         <v>7.7766032569999997</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="14" t="s">
         <v>108</v>
       </c>
@@ -4684,7 +4690,7 @@
         <v>7.78986102</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="14" t="s">
         <v>109</v>
       </c>
@@ -4730,7 +4736,7 @@
         <v>7.8498769999999496E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="14" t="s">
         <v>110</v>
       </c>
@@ -4744,7 +4750,7 @@
         <v>7.7917906620000004</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="14" t="s">
         <v>111</v>
       </c>
@@ -4758,7 +4764,7 @@
         <v>7.7886460780000002</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="14" t="s">
         <v>112</v>
       </c>
@@ -4776,7 +4782,7 @@
       <c r="L103" s="15"/>
       <c r="M103" s="15"/>
     </row>
-    <row r="104" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="14" t="s">
         <v>147</v>
       </c>
@@ -4822,7 +4828,7 @@
         <v>8.5959990000006314E-3</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="14" t="s">
         <v>148</v>
       </c>
@@ -4836,7 +4842,7 @@
         <v>7.6605760270000003</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="14" t="s">
         <v>149</v>
       </c>
@@ -4850,7 +4856,7 @@
         <v>7.6567980359999996</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="14" t="s">
         <v>150</v>
       </c>
@@ -4896,7 +4902,7 @@
         <v>2.3951330000002713E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="14" t="s">
         <v>151</v>
       </c>
@@ -4910,7 +4916,7 @@
         <v>7.6343832159999998</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="14" t="s">
         <v>152</v>
       </c>
@@ -4924,7 +4930,7 @@
         <v>7.6326811010000002</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="14" t="s">
         <v>153</v>
       </c>
@@ -4938,7 +4944,7 @@
         <v>7.6821010679999997</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="14" t="s">
         <v>154</v>
       </c>
@@ -4984,7 +4990,7 @@
         <v>6.1391809999999936E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="14" t="s">
         <v>155</v>
       </c>
@@ -4998,7 +5004,7 @@
         <v>7.1364007689999998</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="14" t="s">
         <v>156</v>
       </c>
@@ -5012,7 +5018,7 @@
         <v>7.1419704160000004</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="14" t="s">
         <v>157</v>
       </c>
@@ -5058,7 +5064,7 @@
         <v>4.2606100000002201E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="14" t="s">
         <v>158</v>
       </c>
@@ -5072,7 +5078,7 @@
         <v>7.468608819</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="14" t="s">
         <v>159</v>
       </c>
@@ -5086,7 +5092,7 @@
         <v>7.4689537149999996</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="14" t="s">
         <v>160</v>
       </c>
@@ -5100,7 +5106,7 @@
         <v>7.6803900140000003</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="14" t="s">
         <v>161</v>
       </c>
@@ -5146,7 +5152,7 @@
         <v>4.6619300000028119E-4</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="14" t="s">
         <v>162</v>
       </c>
@@ -5160,7 +5166,7 @@
         <v>7.667210173</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="14" t="s">
         <v>163</v>
       </c>
@@ -5174,7 +5180,7 @@
         <v>7.6669448720000002</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="14" t="s">
         <v>164</v>
       </c>
@@ -5220,7 +5226,7 @@
         <v>3.2636009999995608E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="14" t="s">
         <v>165</v>
       </c>
@@ -5234,7 +5240,7 @@
         <v>7.6536444919999997</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="14" t="s">
         <v>166</v>
       </c>
@@ -5248,7 +5254,7 @@
         <v>7.653440131</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="14" t="s">
         <v>167</v>
       </c>
@@ -5294,7 +5300,7 @@
         <v>9.8320349999996282E-3</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="14" t="s">
         <v>168</v>
       </c>
@@ -5308,7 +5314,7 @@
         <v>6.3709340689999996</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="14" t="s">
         <v>169</v>
       </c>
@@ -5322,7 +5328,7 @@
         <v>6.3726452409999998</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="21" t="s">
         <v>170</v>
       </c>
@@ -5337,7 +5343,7 @@
         <v>6.9959126630000004</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="14" t="s">
         <v>171</v>
       </c>
@@ -5351,7 +5357,7 @@
         <v>7.6741815879999997</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="14" t="s">
         <v>172</v>
       </c>
@@ -5397,7 +5403,7 @@
         <v>1.8427900000004271E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="14" t="s">
         <v>173</v>
       </c>
@@ -5411,7 +5417,7 @@
         <v>7.6514540369999997</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="14" t="s">
         <v>174</v>
       </c>
@@ -5425,7 +5431,7 @@
         <v>7.6515557080000001</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="14" t="s">
         <v>175</v>
       </c>
@@ -5439,7 +5445,7 @@
         <v>7.316864421</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="14" t="s">
         <v>176</v>
       </c>
@@ -5453,7 +5459,7 @@
         <v>7.9479927589999999</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="14" t="s">
         <v>177</v>
       </c>
@@ -5467,7 +5473,7 @@
         <v>7.6949174229999997</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="14" t="s">
         <v>178</v>
       </c>
@@ -5513,7 +5519,7 @@
         <v>1.1478880999999497E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="14" t="s">
         <v>179</v>
       </c>
@@ -5527,7 +5533,7 @@
         <v>7.6843401650000001</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="14" t="s">
         <v>180</v>
       </c>
@@ -5541,7 +5547,7 @@
         <v>7.6786753970000001</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="14" t="s">
         <v>181</v>
       </c>
@@ -5587,7 +5593,7 @@
         <v>8.2871080000002095E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="14" t="s">
         <v>182</v>
       </c>
@@ -5601,7 +5607,7 @@
         <v>7.6961760779999997</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="14" t="s">
         <v>183</v>
       </c>
@@ -5615,7 +5621,7 @@
         <v>7.6928150100000003</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="14" t="s">
         <v>184</v>
       </c>
@@ -5661,7 +5667,7 @@
         <v>1.2653816000000262E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="14" t="s">
         <v>185</v>
       </c>
@@ -5675,7 +5681,7 @@
         <v>7.6982832630000004</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="14" t="s">
         <v>186</v>
       </c>
@@ -5689,7 +5695,7 @@
         <v>7.7082846360000001</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="14" t="s">
         <v>187</v>
       </c>
@@ -5703,7 +5709,7 @@
         <v>7.7066703499999996</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="14" t="s">
         <v>188</v>
       </c>
@@ -5752,7 +5758,7 @@
         <v>3.4653467921295089E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="14" t="s">
         <v>189</v>
       </c>
@@ -5769,7 +5775,7 @@
         <v>7.9539157263998002</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="14" t="s">
         <v>190</v>
       </c>
@@ -5786,7 +5792,7 @@
         <v>7.9573810731919297</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="14" t="s">
         <v>191</v>
       </c>
@@ -5835,7 +5841,7 @@
         <v>5.9682269996397252E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="14" t="s">
         <v>192</v>
       </c>
@@ -5852,7 +5858,7 @@
         <v>8.0261779270012301</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="14" t="s">
         <v>193</v>
       </c>
@@ -5869,7 +5875,7 @@
         <v>8.0209223405981191</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="14" t="s">
         <v>194</v>
       </c>
@@ -5918,7 +5924,7 @@
         <v>9.7571513074896643E-3</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="14" t="s">
         <v>195</v>
       </c>
@@ -5935,7 +5941,7 @@
         <v>8.0421553587913301</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="14" t="s">
         <v>196</v>
       </c>
@@ -5952,7 +5958,7 @@
         <v>8.0358138115455393</v>
       </c>
     </row>
-    <row r="154" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="14" t="s">
         <v>239</v>
       </c>
@@ -5969,7 +5975,7 @@
         <v>7.67031134315069</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="14" t="s">
         <v>197</v>
       </c>
@@ -5986,7 +5992,7 @@
         <v>8.0745769128785891</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="14" t="s">
         <v>198</v>
       </c>
@@ -6035,7 +6041,7 @@
         <v>4.4601793764700304E-3</v>
       </c>
     </row>
-    <row r="157" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="14" t="s">
         <v>199</v>
       </c>
@@ -6052,7 +6058,7 @@
         <v>7.6355414113303102</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="14" t="s">
         <v>200</v>
       </c>
@@ -6069,7 +6075,7 @@
         <v>7.6379501987185598</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="14" t="s">
         <v>240</v>
       </c>
@@ -6086,7 +6092,7 @@
         <v>7.6830802104558602</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="14" t="s">
         <v>201</v>
       </c>
@@ -6135,7 +6141,7 @@
         <v>2.6236773498995447E-3</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="14" t="s">
         <v>202</v>
       </c>
@@ -6152,7 +6158,7 @@
         <v>7.6469616334670096</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="14" t="s">
         <v>203</v>
       </c>
@@ -6169,7 +6175,7 @@
         <v>7.6495853108169101</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A163" s="14" t="s">
         <v>204</v>
       </c>
@@ -6189,7 +6195,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A164" s="14" t="s">
         <v>205</v>
       </c>
@@ -6209,7 +6215,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="14" t="s">
         <v>208</v>
       </c>
@@ -6255,7 +6261,7 @@
         <v>3.8811856922595922E-3</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="14" t="s">
         <v>209</v>
       </c>
@@ -6269,7 +6275,7 @@
         <v>7.8158333436642904</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="14" t="s">
         <v>210</v>
       </c>
@@ -6315,7 +6321,7 @@
         <v>6.0021903599061233E-4</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="14" t="s">
         <v>211</v>
       </c>
@@ -6329,7 +6335,7 @@
         <v>7.8559850453043403</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="14" t="s">
         <v>212</v>
       </c>
@@ -6375,7 +6381,7 @@
         <v>6.8963092720952801E-4</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="14" t="s">
         <v>213</v>
       </c>
@@ -6389,7 +6395,7 @@
         <v>7.8611367023104597</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="14" t="s">
         <v>214</v>
       </c>
@@ -6435,7 +6441,7 @@
         <v>2.3053612821302139E-3</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="14" t="s">
         <v>215</v>
       </c>
@@ -6449,7 +6455,7 @@
         <v>7.8656749752011397</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="14" t="s">
         <v>225</v>
       </c>
@@ -6467,7 +6473,7 @@
       <c r="L173" s="15"/>
       <c r="M173" s="15"/>
     </row>
-    <row r="174" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="14" t="s">
         <v>216</v>
       </c>
@@ -6513,7 +6519,7 @@
         <v>1.6735989730900513E-3</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="14" t="s">
         <v>217</v>
       </c>
@@ -6527,7 +6533,7 @@
         <v>7.8658232744760301</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="14" t="s">
         <v>218</v>
       </c>
@@ -6573,7 +6579,7 @@
         <v>1.5296409123903842E-3</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="14" t="s">
         <v>219</v>
       </c>
@@ -6587,7 +6593,7 @@
         <v>7.7910625496787098</v>
       </c>
     </row>
-    <row r="178" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="14" t="s">
         <v>220</v>
       </c>
@@ -6633,7 +6639,7 @@
         <v>6.2976206001152946E-6</v>
       </c>
     </row>
-    <row r="179" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="14" t="s">
         <v>221</v>
       </c>
@@ -6647,7 +6653,7 @@
         <v>7.77674822365426</v>
       </c>
     </row>
-    <row r="180" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="14" t="s">
         <v>222</v>
       </c>
@@ -6696,7 +6702,7 @@
         <v>0.13822254951569946</v>
       </c>
     </row>
-    <row r="181" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="14" t="s">
         <v>223</v>
       </c>
@@ -6713,7 +6719,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="182" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="14" t="s">
         <v>226</v>
       </c>
@@ -6730,7 +6736,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="183" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="14" t="s">
         <v>224</v>
       </c>
@@ -6744,7 +6750,7 @@
         <v>7.86089245271185</v>
       </c>
     </row>
-    <row r="184" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="14" t="s">
         <v>226</v>
       </c>
@@ -6762,7 +6768,7 @@
       <c r="L184" s="15"/>
       <c r="M184" s="15"/>
     </row>
-    <row r="185" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="14" t="s">
         <v>227</v>
       </c>
@@ -6808,7 +6814,7 @@
         <v>1.7011204008694492E-3</v>
       </c>
     </row>
-    <row r="186" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="14" t="s">
         <v>228</v>
       </c>
@@ -6822,7 +6828,7 @@
         <v>7.8202712500762397</v>
       </c>
     </row>
-    <row r="187" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="14" t="s">
         <v>229</v>
       </c>
@@ -6868,7 +6874,7 @@
         <v>2.9082277420729774E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="14" t="s">
         <v>230</v>
       </c>
@@ -6882,7 +6888,7 @@
         <v>7.87404002677488</v>
       </c>
     </row>
-    <row r="189" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="14" t="s">
         <v>231</v>
       </c>
@@ -6928,7 +6934,7 @@
         <v>2.6729756152799489E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="14" t="s">
         <v>232</v>
       </c>
@@ -6942,7 +6948,7 @@
         <v>7.8471181750488697</v>
       </c>
     </row>
-    <row r="191" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="14" t="s">
         <v>233</v>
       </c>
@@ -6988,7 +6994,7 @@
         <v>5.3888669986097426E-3</v>
       </c>
     </row>
-    <row r="192" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="14" t="s">
         <v>234</v>
       </c>
@@ -7002,7 +7008,7 @@
         <v>7.7813583054262701</v>
       </c>
     </row>
-    <row r="193" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="14" t="s">
         <v>247</v>
       </c>
@@ -7048,7 +7054,7 @@
         <v>2.8102638491498411E-3</v>
       </c>
     </row>
-    <row r="194" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="14" t="s">
         <v>248</v>
       </c>
@@ -7062,7 +7068,7 @@
         <v>7.7568912448131098</v>
       </c>
     </row>
-    <row r="195" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="14" t="s">
         <v>249</v>
       </c>
@@ -7108,7 +7114,7 @@
         <v>1.9084552613604089E-3</v>
       </c>
     </row>
-    <row r="196" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="14" t="s">
         <v>250</v>
       </c>
@@ -7122,7 +7128,7 @@
         <v>7.8733900677320703</v>
       </c>
     </row>
-    <row r="197" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="14" t="s">
         <v>251</v>
       </c>
@@ -7168,7 +7174,7 @@
         <v>2.0846582444002948E-3</v>
       </c>
     </row>
-    <row r="198" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="14" t="s">
         <v>252</v>
       </c>
@@ -7182,7 +7188,7 @@
         <v>7.7263978191714298</v>
       </c>
     </row>
-    <row r="199" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="14" t="s">
         <v>253</v>
       </c>
@@ -7228,7 +7234,7 @@
         <v>3.3138559194894057E-3</v>
       </c>
     </row>
-    <row r="200" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="14" t="s">
         <v>254</v>
       </c>
@@ -7242,7 +7248,7 @@
         <v>7.7624872040259403</v>
       </c>
     </row>
-    <row r="201" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="14" t="s">
         <v>264</v>
       </c>
@@ -7256,7 +7262,7 @@
         <v>7.7065716469648402</v>
       </c>
     </row>
-    <row r="202" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="14" t="s">
         <v>255</v>
       </c>
@@ -7302,7 +7308,7 @@
         <v>2.4641745023901152E-3</v>
       </c>
     </row>
-    <row r="203" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="14" t="s">
         <v>256</v>
       </c>
@@ -7316,7 +7322,7 @@
         <v>7.7295066813725404</v>
       </c>
     </row>
-    <row r="204" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="14" t="s">
         <v>257</v>
       </c>
@@ -7362,7 +7368,7 @@
         <v>1.8364403182902223E-3</v>
       </c>
     </row>
-    <row r="205" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="14" t="s">
         <v>258</v>
       </c>
@@ -7376,7 +7382,7 @@
         <v>7.7135628084406003</v>
       </c>
     </row>
-    <row r="206" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="14" t="s">
         <v>259</v>
       </c>
@@ -7422,7 +7428,7 @@
         <v>7.1404976746798354E-3</v>
       </c>
     </row>
-    <row r="207" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="14" t="s">
         <v>260</v>
       </c>
@@ -7436,7 +7442,7 @@
         <v>7.78548679949935</v>
       </c>
     </row>
-    <row r="208" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="14" t="s">
         <v>261</v>
       </c>
@@ -7482,7 +7488,7 @@
         <v>1.5627490742886607E-3</v>
       </c>
     </row>
-    <row r="209" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="14" t="s">
         <v>262</v>
       </c>
@@ -7496,7 +7502,7 @@
         <v>7.9116433615381201</v>
       </c>
     </row>
-    <row r="210" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="14" t="s">
         <v>263</v>
       </c>
@@ -7510,7 +7516,7 @@
         <v>7.7210421811258003</v>
       </c>
     </row>
-    <row r="211" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A211" s="14" t="s">
         <v>265</v>
       </c>
@@ -7559,7 +7565,7 @@
         <v>0.1854344769760301</v>
       </c>
     </row>
-    <row r="212" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A212" s="14" t="s">
         <v>266</v>
       </c>
@@ -7576,7 +7582,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="213" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A213" s="14" t="s">
         <v>267</v>
       </c>
@@ -7625,7 +7631,7 @@
         <v>0.19568697425110049</v>
       </c>
     </row>
-    <row r="214" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A214" s="14" t="s">
         <v>268</v>
       </c>
@@ -7642,7 +7648,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="215" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A215" s="14" t="s">
         <v>269</v>
       </c>
@@ -7691,7 +7697,7 @@
         <v>3.6690036611499721E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A216" s="14" t="s">
         <v>270</v>
       </c>
@@ -7708,7 +7714,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="217" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A217" s="14" t="s">
         <v>271</v>
       </c>
@@ -7757,7 +7763,7 @@
         <v>2.9172948538660037E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A218" s="14" t="s">
         <v>272</v>
       </c>
@@ -7774,7 +7780,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="219" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A219" s="14" t="s">
         <v>273</v>
       </c>
@@ -7791,7 +7797,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="220" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A220" s="14" t="s">
         <v>275</v>
       </c>
@@ -7840,7 +7846,7 @@
         <v>7.1857585881370589E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A221" s="14" t="s">
         <v>276</v>
       </c>
@@ -7857,7 +7863,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="222" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A222" s="14" t="s">
         <v>277</v>
       </c>
@@ -7906,7 +7912,7 @@
         <v>5.7847597330809464E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A223" s="14" t="s">
         <v>278</v>
       </c>
@@ -7923,7 +7929,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="224" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A224" s="14" t="s">
         <v>279</v>
       </c>
@@ -7972,7 +7978,7 @@
         <v>0.2161789027148604</v>
       </c>
     </row>
-    <row r="225" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A225" s="14" t="s">
         <v>280</v>
       </c>
@@ -7989,7 +7995,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="226" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A226" s="14" t="s">
         <v>281</v>
       </c>
@@ -8038,7 +8044,7 @@
         <v>3.847784957223066E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A227" s="14" t="s">
         <v>282</v>
       </c>
@@ -8055,7 +8061,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="228" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A228" s="14" t="s">
         <v>283</v>
       </c>
@@ -8072,7 +8078,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="229" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="14" t="s">
         <v>284</v>
       </c>
@@ -8118,7 +8124,7 @@
         <v>9.2158552030479512E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="14" t="s">
         <v>285</v>
       </c>
@@ -8132,7 +8138,7 @@
         <v>7.6791676929657999</v>
       </c>
     </row>
-    <row r="231" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="14" t="s">
         <v>286</v>
       </c>
@@ -8178,7 +8184,7 @@
         <v>1.6493493007419424E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="14" t="s">
         <v>287</v>
       </c>
@@ -8192,7 +8198,7 @@
         <v>7.6709188894545699</v>
       </c>
     </row>
-    <row r="233" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="14" t="s">
         <v>288</v>
       </c>
@@ -8238,7 +8244,7 @@
         <v>2.514442181299259E-3</v>
       </c>
     </row>
-    <row r="234" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="14" t="s">
         <v>289</v>
       </c>
@@ -8252,7 +8258,7 @@
         <v>7.8598848256278</v>
       </c>
     </row>
-    <row r="235" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="14" t="s">
         <v>290</v>
       </c>
@@ -8298,7 +8304,7 @@
         <v>2.7849821903496164E-3</v>
       </c>
     </row>
-    <row r="236" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="14" t="s">
         <v>291</v>
       </c>
@@ -8312,7 +8318,7 @@
         <v>7.8379624344456804</v>
       </c>
     </row>
-    <row r="237" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="14" t="s">
         <v>292</v>
       </c>
@@ -8358,7 +8364,7 @@
         <v>5.5981880994604438E-3</v>
       </c>
     </row>
-    <row r="238" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="14" t="s">
         <v>293</v>
       </c>
@@ -8372,7 +8378,7 @@
         <v>7.87093476212707</v>
       </c>
     </row>
-    <row r="239" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="14" t="s">
         <v>294</v>
       </c>
@@ -8418,7 +8424,7 @@
         <v>5.392089089202301E-4</v>
       </c>
     </row>
-    <row r="240" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="14" t="s">
         <v>295</v>
       </c>
@@ -8432,7 +8438,7 @@
         <v>7.8838242011011399</v>
       </c>
     </row>
-    <row r="241" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="14" t="s">
         <v>296</v>
       </c>
@@ -8446,7 +8452,7 @@
         <v>8.1335197047369494</v>
       </c>
     </row>
-    <row r="242" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="14" t="s">
         <v>297</v>
       </c>
@@ -8492,7 +8498,7 @@
         <v>3.1388050428500236E-3</v>
       </c>
     </row>
-    <row r="243" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="14" t="s">
         <v>298</v>
       </c>
@@ -8506,7 +8512,7 @@
         <v>7.715093927551</v>
       </c>
     </row>
-    <row r="244" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="14" t="s">
         <v>299</v>
       </c>
@@ -8520,7 +8526,7 @@
         <v>7.71823273259385</v>
       </c>
     </row>
-    <row r="245" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="14" t="s">
         <v>300</v>
       </c>
@@ -8534,7 +8540,7 @@
         <v>7.7164851704236099</v>
       </c>
     </row>
-    <row r="246" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="14" t="s">
         <v>301</v>
       </c>
@@ -8548,7 +8554,7 @@
         <v>7.7176880414598603</v>
       </c>
     </row>
-    <row r="247" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="14" t="s">
         <v>302</v>
       </c>
@@ -8562,7 +8568,7 @@
         <v>7.7176845907370097</v>
       </c>
     </row>
-    <row r="248" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="14" t="s">
         <v>303</v>
       </c>
@@ -8576,7 +8582,7 @@
         <v>7.7177699275983898</v>
       </c>
     </row>
-    <row r="249" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="14" t="s">
         <v>304</v>
       </c>
@@ -8622,7 +8628,7 @@
         <v>2.868591346249616E-3</v>
       </c>
     </row>
-    <row r="250" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="14" t="s">
         <v>305</v>
       </c>
@@ -8636,7 +8642,7 @@
         <v>7.8910532349370897</v>
       </c>
     </row>
-    <row r="251" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="14" t="s">
         <v>306</v>
       </c>
@@ -8650,7 +8656,7 @@
         <v>7.8886622600254999</v>
       </c>
     </row>
-    <row r="252" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="14" t="s">
         <v>307</v>
       </c>
@@ -8696,7 +8702,7 @@
         <v>2.2397760814900636E-3</v>
       </c>
     </row>
-    <row r="253" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="14" t="s">
         <v>308</v>
       </c>
@@ -8710,7 +8716,7 @@
         <v>7.8245624615943301</v>
       </c>
     </row>
-    <row r="254" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="14" t="s">
         <v>309</v>
       </c>
@@ -8724,7 +8730,7 @@
         <v>7.8242606687707301</v>
       </c>
     </row>
-    <row r="255" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="14" t="s">
         <v>310</v>
       </c>
@@ -8770,7 +8776,7 @@
         <v>4.6256493783394248E-3</v>
       </c>
     </row>
-    <row r="256" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="14" t="s">
         <v>311</v>
       </c>
@@ -8784,7 +8790,7 @@
         <v>7.7863432043211098</v>
       </c>
     </row>
-    <row r="257" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="14" t="s">
         <v>312</v>
       </c>
@@ -8798,7 +8804,7 @@
         <v>7.7832724143483096</v>
       </c>
     </row>
-    <row r="258" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="14" t="s">
         <v>313</v>
       </c>
@@ -8812,7 +8818,7 @@
         <v>7.7259869711707596</v>
       </c>
     </row>
-    <row r="259" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="14" t="s">
         <v>315</v>
       </c>
@@ -8858,7 +8864,7 @@
         <v>8.4773166248002241E-3</v>
       </c>
     </row>
-    <row r="260" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="14" t="s">
         <v>317</v>
       </c>
@@ -8872,7 +8878,7 @@
         <v>7.7031565218517004</v>
       </c>
     </row>
-    <row r="261" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" s="14" t="s">
         <v>314</v>
       </c>
@@ -8886,7 +8892,7 @@
         <v>7.6949378745119601</v>
       </c>
     </row>
-    <row r="262" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A262" s="14" t="s">
         <v>316</v>
       </c>
@@ -8900,7 +8906,7 @@
         <v>7.7034151911367603</v>
       </c>
     </row>
-    <row r="263" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A263" s="14" t="s">
         <v>334</v>
       </c>
@@ -8914,7 +8920,7 @@
         <v>7.7577451759517997</v>
       </c>
     </row>
-    <row r="264" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" s="14" t="s">
         <v>335</v>
       </c>
@@ -8963,7 +8969,7 @@
         <v>8.6420170405330232E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" s="14" t="s">
         <v>336</v>
       </c>
@@ -8980,7 +8986,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="266" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A266" s="14" t="s">
         <v>337</v>
       </c>
@@ -8997,7 +9003,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="267" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" s="14" t="s">
         <v>338</v>
       </c>
@@ -9046,7 +9052,7 @@
         <v>1.5990523893796293E-3</v>
       </c>
     </row>
-    <row r="268" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="14" t="s">
         <v>339</v>
       </c>
@@ -9063,7 +9069,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="269" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="14" t="s">
         <v>340</v>
       </c>
@@ -9080,7 +9086,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="270" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" s="14" t="s">
         <v>341</v>
       </c>
@@ -9129,7 +9135,7 @@
         <v>3.4933230606680077E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A271" s="14" t="s">
         <v>342</v>
       </c>
@@ -9146,7 +9152,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="272" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A272" s="14" t="s">
         <v>319</v>
       </c>
@@ -9195,7 +9201,7 @@
         <v>3.5188640498500234E-3</v>
       </c>
     </row>
-    <row r="273" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A273" s="14" t="s">
         <v>320</v>
       </c>
@@ -9209,7 +9215,7 @@
         <v>8.0920518190004298</v>
       </c>
     </row>
-    <row r="274" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" s="14" t="s">
         <v>321</v>
       </c>
@@ -9223,7 +9229,7 @@
         <v>8.0914101715023303</v>
       </c>
     </row>
-    <row r="275" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A275" s="14" t="s">
         <v>322</v>
       </c>
@@ -9269,7 +9275,7 @@
         <v>7.5741192992895279E-3</v>
       </c>
     </row>
-    <row r="276" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" s="14" t="s">
         <v>323</v>
       </c>
@@ -9286,7 +9292,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="277" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A277" s="14" t="s">
         <v>324</v>
       </c>
@@ -9303,7 +9309,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="278" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A278" s="14" t="s">
         <v>325</v>
       </c>
@@ -9349,7 +9355,7 @@
         <v>1.5070709635303103E-3</v>
       </c>
     </row>
-    <row r="279" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A279" s="14" t="s">
         <v>326</v>
       </c>
@@ -9363,7 +9369,7 @@
         <v>7.8382903790055503</v>
       </c>
     </row>
-    <row r="280" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A280" s="14" t="s">
         <v>327</v>
       </c>
@@ -9377,7 +9383,7 @@
         <v>7.8375542649159202</v>
       </c>
     </row>
-    <row r="281" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A281" s="14" t="s">
         <v>344</v>
       </c>
@@ -9394,7 +9400,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="282" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A282" s="14" t="s">
         <v>345</v>
       </c>
@@ -9443,7 +9449,7 @@
         <v>2.3715898049670336E-2</v>
       </c>
     </row>
-    <row r="283" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A283" s="14" t="s">
         <v>346</v>
       </c>
@@ -9460,7 +9466,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="284" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A284" s="14" t="s">
         <v>347</v>
       </c>
@@ -9509,7 +9515,7 @@
         <v>1.4793985413700028E-2</v>
       </c>
     </row>
-    <row r="285" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A285" s="14" t="s">
         <v>348</v>
       </c>
@@ -9526,7 +9532,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="286" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" s="14" t="s">
         <v>349</v>
       </c>
@@ -9575,7 +9581,7 @@
         <v>1.5195024406249757E-2</v>
       </c>
     </row>
-    <row r="287" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A287" s="14" t="s">
         <v>350</v>
       </c>
@@ -9592,7 +9598,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="288" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A288" s="14" t="s">
         <v>351</v>
       </c>
@@ -9641,7 +9647,7 @@
         <v>1.161899045510939E-2</v>
       </c>
     </row>
-    <row r="289" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A289" s="14" t="s">
         <v>352</v>
       </c>
@@ -9658,7 +9664,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="290" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A290" s="14" t="s">
         <v>344</v>
       </c>
@@ -9672,7 +9678,7 @@
         <v>7.8537609950039702</v>
       </c>
     </row>
-    <row r="291" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A291" s="14" t="s">
         <v>355</v>
       </c>
@@ -9721,7 +9727,7 @@
         <v>2.6480046440102711E-3</v>
       </c>
     </row>
-    <row r="292" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A292" s="14" t="s">
         <v>356</v>
       </c>
@@ -9738,7 +9744,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="293" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" s="14" t="s">
         <v>357</v>
       </c>
@@ -9787,7 +9793,7 @@
         <v>8.280416818591263E-4</v>
       </c>
     </row>
-    <row r="294" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A294" s="14" t="s">
         <v>358</v>
       </c>
@@ -9804,7 +9810,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="295" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A295" s="14" t="s">
         <v>359</v>
       </c>
@@ -9853,7 +9859,7 @@
         <v>1.3811298887134171E-4</v>
       </c>
     </row>
-    <row r="296" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A296" s="14" t="s">
         <v>360</v>
       </c>
@@ -9870,7 +9876,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="297" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A297" s="14" t="s">
         <v>361</v>
       </c>
@@ -9919,7 +9925,7 @@
         <v>6.3001943405600613E-3</v>
       </c>
     </row>
-    <row r="298" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A298" s="14" t="s">
         <v>362</v>
       </c>
@@ -9936,7 +9942,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="299" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A299" s="14" t="s">
         <v>344</v>
       </c>
@@ -9950,7 +9956,7 @@
         <v>7.8312402209114502</v>
       </c>
     </row>
-    <row r="300" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A300" s="14" t="s">
         <v>363</v>
       </c>
@@ -9999,7 +10005,7 @@
         <v>1.5636857043999086E-3</v>
       </c>
     </row>
-    <row r="301" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A301" s="14" t="s">
         <v>364</v>
       </c>
@@ -10016,7 +10022,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="302" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A302" s="14" t="s">
         <v>365</v>
       </c>
@@ -10065,7 +10071,7 @@
         <v>1.7880607543805382E-3</v>
       </c>
     </row>
-    <row r="303" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A303" s="14" t="s">
         <v>366</v>
       </c>
@@ -10082,7 +10088,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="304" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A304" s="14" t="s">
         <v>367</v>
       </c>
@@ -10131,7 +10137,7 @@
         <v>7.9761327169194374E-3</v>
       </c>
     </row>
-    <row r="305" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A305" s="14" t="s">
         <v>368</v>
       </c>
@@ -10148,7 +10154,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="306" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A306" s="14" t="s">
         <v>369</v>
       </c>
@@ -10197,7 +10203,7 @@
         <v>3.2952516978594915E-3</v>
       </c>
     </row>
-    <row r="307" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A307" s="14" t="s">
         <v>370</v>
       </c>
@@ -10214,7 +10220,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="308" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A308" s="14" t="s">
         <v>344</v>
       </c>
@@ -10228,7 +10234,7 @@
         <v>7.8391823136575702</v>
       </c>
     </row>
-    <row r="309" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A309" s="14" t="s">
         <v>371</v>
       </c>
@@ -10277,7 +10283,7 @@
         <v>7.549687215099965E-3</v>
       </c>
     </row>
-    <row r="310" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A310" s="14" t="s">
         <v>372</v>
       </c>
@@ -10294,7 +10300,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="311" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A311" s="14" t="s">
         <v>373</v>
       </c>
@@ -10343,7 +10349,7 @@
         <v>4.7754687428698261E-3</v>
       </c>
     </row>
-    <row r="312" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A312" s="14" t="s">
         <v>374</v>
       </c>
@@ -10360,7 +10366,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="313" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A313" s="14" t="s">
         <v>375</v>
       </c>
@@ -10409,7 +10415,7 @@
         <v>1.746508977630512E-3</v>
       </c>
     </row>
-    <row r="314" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A314" s="14" t="s">
         <v>376</v>
       </c>
@@ -10426,7 +10432,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="315" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A315" s="14" t="s">
         <v>377</v>
       </c>
@@ -10475,7 +10481,7 @@
         <v>1.3990524056409548E-2</v>
       </c>
     </row>
-    <row r="316" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A316" s="14" t="s">
         <v>378</v>
       </c>
@@ -10489,6 +10495,86 @@
         <v>7.7525382359909099</v>
       </c>
       <c r="F316" s="16" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="317" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A317" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="B317" s="18">
+        <v>44356</v>
+      </c>
+      <c r="D317" s="15">
+        <v>7.9882060711433303</v>
+      </c>
+      <c r="E317" s="15">
+        <v>7.8298160240183803</v>
+      </c>
+    </row>
+    <row r="318" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A318" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="B318" s="18">
+        <v>44356</v>
+      </c>
+      <c r="D318" s="15">
+        <v>7.87301497535476</v>
+      </c>
+      <c r="E318" s="15">
+        <v>7.7317662543351897</v>
+      </c>
+      <c r="F318" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G318" s="15">
+        <f>AVERAGE(D318:D319)</f>
+        <v>7.8704614600286202</v>
+      </c>
+      <c r="H318" s="14">
+        <f>_xlfn.STDEV.S(D318:D319)</f>
+        <v>3.6112160059550737E-3</v>
+      </c>
+      <c r="I318" s="14">
+        <f>2*H318</f>
+        <v>7.2224320119101473E-3</v>
+      </c>
+      <c r="J318" s="14">
+        <f>H318/G318</f>
+        <v>4.588315468279978E-4</v>
+      </c>
+      <c r="K318" s="19">
+        <f>J318</f>
+        <v>4.588315468279978E-4</v>
+      </c>
+      <c r="L318" s="15">
+        <f>MIN(D318:D319)</f>
+        <v>7.8679079447024796</v>
+      </c>
+      <c r="M318" s="15">
+        <f>MAX(D318:D319)</f>
+        <v>7.87301497535476</v>
+      </c>
+      <c r="N318" s="14">
+        <f>M318-L318</f>
+        <v>5.1070306522804643E-3</v>
+      </c>
+    </row>
+    <row r="319" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A319" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="B319" s="18">
+        <v>44356</v>
+      </c>
+      <c r="D319" s="15">
+        <v>7.8679079447024796</v>
+      </c>
+      <c r="E319" s="15">
+        <v>7.7268089866402896</v>
+      </c>
+      <c r="F319" s="16" t="s">
         <v>343</v>
       </c>
     </row>
@@ -10511,25 +10597,25 @@
       <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="103" style="6" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.5703125" style="9" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.5546875" style="9" customWidth="1"/>
+    <col min="14" max="14" width="14.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>40</v>
       </c>
@@ -10563,7 +10649,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>53</v>
       </c>
@@ -10600,7 +10686,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>61</v>
       </c>
@@ -10627,7 +10713,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>77</v>
       </c>
@@ -10657,7 +10743,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>95</v>
       </c>
@@ -10690,7 +10776,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>98</v>
       </c>
@@ -10720,7 +10806,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>102</v>
       </c>
@@ -10740,7 +10826,7 @@
         <v>1.4675794477244731E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>130</v>
       </c>
@@ -10760,7 +10846,7 @@
         <v>9.5489994253788926E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>112</v>
       </c>
@@ -10780,7 +10866,7 @@
         <v>1.516738390249465E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>197</v>
       </c>
@@ -10800,7 +10886,7 @@
         <v>3.5994366965510827E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
         <v>296</v>
       </c>
@@ -10820,7 +10906,7 @@
         <v>1.5976496949771635E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>330</v>
       </c>
@@ -10840,37 +10926,37 @@
         <v>5.6563284241221383E-7</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="24"/>
       <c r="B13" s="25"/>
       <c r="C13" s="26"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="24"/>
       <c r="B14" s="25"/>
       <c r="C14" s="26"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="24"/>
       <c r="B15" s="25"/>
       <c r="C15" s="26"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="24"/>
       <c r="B16" s="25"/>
       <c r="C16" s="26"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="24"/>
       <c r="B17" s="25"/>
       <c r="C17" s="26"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="24"/>
       <c r="B18" s="25"/>
       <c r="C18" s="26"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="24"/>
       <c r="B19" s="25"/>
       <c r="C19" s="26"/>
@@ -10881,7 +10967,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="24"/>
       <c r="B20" s="25"/>
       <c r="C20" s="26"/>
@@ -10892,147 +10978,147 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="24"/>
       <c r="B21" s="25"/>
       <c r="C21" s="26"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="24"/>
       <c r="B22" s="25"/>
       <c r="C22" s="26"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="24"/>
       <c r="B23" s="25"/>
       <c r="C23" s="26"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="24"/>
       <c r="B24" s="25"/>
       <c r="C24" s="26"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="24"/>
       <c r="B25" s="25"/>
       <c r="C25" s="26"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C26" s="26"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C27" s="26"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C28" s="26"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C29" s="26"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C30" s="26"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C31" s="26"/>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C32" s="26"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" s="26"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" s="26"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" s="26"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C36" s="26"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C37" s="26"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C38" s="26"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C39" s="26"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C40" s="26"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C41" s="26"/>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C42" s="26"/>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C43" s="26"/>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C44" s="26"/>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C45" s="26"/>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C46" s="26"/>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C47" s="26"/>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C48" s="26"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C49" s="26"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C50" s="26"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C51" s="26"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C52" s="26"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C53" s="26"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C54" s="26"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C55" s="26"/>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C56" s="26"/>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" s="26"/>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C58" s="26"/>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" s="26"/>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C60" s="26"/>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61" s="26"/>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C62" s="26"/>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C63" s="26"/>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C64" s="26"/>
     </row>
   </sheetData>
@@ -11050,25 +11136,25 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.109375" style="6" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="103" style="6" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" style="9" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="10" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" style="9" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -11102,7 +11188,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>153</v>
       </c>
@@ -11143,7 +11229,7 @@
         <v>11.92</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>160</v>
       </c>
@@ -11184,7 +11270,7 @@
         <v>14.11</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>171</v>
       </c>
@@ -11214,7 +11300,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>177</v>
       </c>
@@ -11244,7 +11330,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>187</v>
       </c>
@@ -11264,7 +11350,7 @@
         <v>6.0364966713408619E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>239</v>
       </c>
@@ -11284,7 +11370,7 @@
         <v>1.3899760750579057E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>240</v>
       </c>
@@ -11304,7 +11390,7 @@
         <v>9.5872032397609086E-7</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>204</v>
       </c>
@@ -11324,7 +11410,7 @@
         <v>2.2764778095089857E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>205</v>
       </c>
@@ -11344,7 +11430,7 @@
         <v>2.5736318323859534E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>225</v>
       </c>
@@ -11364,7 +11450,7 @@
         <v>3.6664135788884965E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>224</v>
       </c>
@@ -11384,7 +11470,7 @@
         <v>3.1966359315675798E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>313</v>
       </c>
@@ -11404,7 +11490,7 @@
         <v>1.9259725139259944E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>329</v>
       </c>
@@ -11424,27 +11510,27 @@
         <v>9.9644047605947084E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
@@ -11455,7 +11541,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C20" s="9"/>
       <c r="F20" s="7" t="s">
         <v>38</v>
@@ -11464,22 +11550,22 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C22" s="9"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C23" s="9"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C24" s="9"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C25" s="9"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F31" s="7"/>
     </row>
   </sheetData>

</xml_diff>